<commit_message>
Update Onboarding And Login Non Private
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Trillia\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\BespokeAPI\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1774A0-6E56-49E3-B3B4-82491BA93DBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3806860E-8FFA-4E67-B932-E021C7598DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin Category" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="1198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="1221">
   <si>
     <t>CategoryNametext</t>
   </si>
@@ -3424,72 +3424,6 @@
     <t>SellerLocation</t>
   </si>
   <si>
-    <t>Seller001</t>
-  </si>
-  <si>
-    <t>Seller002</t>
-  </si>
-  <si>
-    <t>Seller003</t>
-  </si>
-  <si>
-    <t>Seller004</t>
-  </si>
-  <si>
-    <t>Seller005</t>
-  </si>
-  <si>
-    <t>Seller006</t>
-  </si>
-  <si>
-    <t>Seller007</t>
-  </si>
-  <si>
-    <t>Seller008</t>
-  </si>
-  <si>
-    <t>Seller009</t>
-  </si>
-  <si>
-    <t>Seller010</t>
-  </si>
-  <si>
-    <t>Seller011</t>
-  </si>
-  <si>
-    <t>Seller012</t>
-  </si>
-  <si>
-    <t>Seller013</t>
-  </si>
-  <si>
-    <t>Seller014</t>
-  </si>
-  <si>
-    <t>Seller015</t>
-  </si>
-  <si>
-    <t>Seller016</t>
-  </si>
-  <si>
-    <t>Seller017</t>
-  </si>
-  <si>
-    <t>Seller018</t>
-  </si>
-  <si>
-    <t>Seller019</t>
-  </si>
-  <si>
-    <t>Seller020</t>
-  </si>
-  <si>
-    <t>Seller021</t>
-  </si>
-  <si>
-    <t>Seller022</t>
-  </si>
-  <si>
     <t>seller_goldwyn1@yopmail.com</t>
   </si>
   <si>
@@ -3632,6 +3566,141 @@
   </si>
   <si>
     <t>buyer_rtbukater1@yopmail.com</t>
+  </si>
+  <si>
+    <t>Seller0001</t>
+  </si>
+  <si>
+    <t>Seller0002</t>
+  </si>
+  <si>
+    <t>Seller0003</t>
+  </si>
+  <si>
+    <t>Seller0004</t>
+  </si>
+  <si>
+    <t>Seller0005</t>
+  </si>
+  <si>
+    <t>Seller0006</t>
+  </si>
+  <si>
+    <t>Seller0007</t>
+  </si>
+  <si>
+    <t>Seller0008</t>
+  </si>
+  <si>
+    <t>Seller0009</t>
+  </si>
+  <si>
+    <t>Seller0010</t>
+  </si>
+  <si>
+    <t>Seller0011</t>
+  </si>
+  <si>
+    <t>Seller0012</t>
+  </si>
+  <si>
+    <t>Seller0013</t>
+  </si>
+  <si>
+    <t>Seller0014</t>
+  </si>
+  <si>
+    <t>Seller0015</t>
+  </si>
+  <si>
+    <t>Seller0016</t>
+  </si>
+  <si>
+    <t>Seller0017</t>
+  </si>
+  <si>
+    <t>Seller0018</t>
+  </si>
+  <si>
+    <t>Seller0019</t>
+  </si>
+  <si>
+    <t>Seller0020</t>
+  </si>
+  <si>
+    <t>Seller0021</t>
+  </si>
+  <si>
+    <t>Seller0022</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\1.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\2.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\3.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\4.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\5.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\6.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\7.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\8.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\9.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\10.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\11.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\12.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\13.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\14.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\15.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\16.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\17.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\18.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\19.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\20.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\21.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\22.png</t>
+  </si>
+  <si>
+    <t>C:\\Katalon\\BespokeAPI\\Images\\SellerPhoto\\23.png</t>
   </si>
 </sst>
 </file>
@@ -6485,13 +6554,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0C2BDA-D892-4B24-9F47-C0E0D73BE072}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A2:A22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" style="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="62.140625" style="34" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
@@ -6505,7 +6574,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
-        <v>1152</v>
+        <v>1130</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>149</v>
@@ -6552,10 +6621,10 @@
     </row>
     <row r="2" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
-        <v>1153</v>
+        <v>1198</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1128</v>
+        <v>1176</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>160</v>
@@ -6599,10 +6668,10 @@
     </row>
     <row r="3" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
-        <v>1154</v>
+        <v>1199</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1129</v>
+        <v>1177</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>167</v>
@@ -6646,10 +6715,10 @@
     </row>
     <row r="4" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
-        <v>1155</v>
+        <v>1200</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1130</v>
+        <v>1178</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>172</v>
@@ -6691,10 +6760,10 @@
     </row>
     <row r="5" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
-        <v>1156</v>
+        <v>1201</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1131</v>
+        <v>1179</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>177</v>
@@ -6738,10 +6807,10 @@
     </row>
     <row r="6" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
-        <v>1157</v>
+        <v>1202</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1132</v>
+        <v>1180</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>184</v>
@@ -6785,10 +6854,10 @@
     </row>
     <row r="7" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
-        <v>1158</v>
+        <v>1203</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1133</v>
+        <v>1181</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>191</v>
@@ -6832,10 +6901,10 @@
     </row>
     <row r="8" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
-        <v>1159</v>
+        <v>1204</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1134</v>
+        <v>1182</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>197</v>
@@ -6879,10 +6948,10 @@
     </row>
     <row r="9" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
-        <v>1160</v>
+        <v>1205</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1135</v>
+        <v>1183</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>202</v>
@@ -6926,10 +6995,10 @@
     </row>
     <row r="10" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
-        <v>1161</v>
+        <v>1206</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1136</v>
+        <v>1184</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>207</v>
@@ -6973,10 +7042,10 @@
     </row>
     <row r="11" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
-        <v>1162</v>
+        <v>1207</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1137</v>
+        <v>1185</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>211</v>
@@ -7020,10 +7089,10 @@
     </row>
     <row r="12" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
-        <v>1163</v>
+        <v>1208</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1138</v>
+        <v>1186</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>216</v>
@@ -7067,10 +7136,10 @@
     </row>
     <row r="13" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
-        <v>1164</v>
+        <v>1209</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1139</v>
+        <v>1187</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>221</v>
@@ -7114,10 +7183,10 @@
     </row>
     <row r="14" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
-        <v>1165</v>
+        <v>1210</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1140</v>
+        <v>1188</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>226</v>
@@ -7161,10 +7230,10 @@
     </row>
     <row r="15" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
-        <v>1166</v>
+        <v>1211</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1141</v>
+        <v>1189</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>231</v>
@@ -7208,10 +7277,10 @@
     </row>
     <row r="16" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
-        <v>1167</v>
+        <v>1212</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1142</v>
+        <v>1190</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>237</v>
@@ -7255,10 +7324,10 @@
     </row>
     <row r="17" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
-        <v>1168</v>
+        <v>1213</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>1143</v>
+        <v>1191</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>242</v>
@@ -7302,10 +7371,10 @@
     </row>
     <row r="18" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="s">
-        <v>1169</v>
+        <v>1214</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1144</v>
+        <v>1192</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>247</v>
@@ -7349,10 +7418,10 @@
     </row>
     <row r="19" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
-        <v>1170</v>
+        <v>1215</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1145</v>
+        <v>1193</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>252</v>
@@ -7394,10 +7463,10 @@
     </row>
     <row r="20" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32" t="s">
-        <v>1171</v>
+        <v>1216</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>1146</v>
+        <v>1194</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>256</v>
@@ -7439,10 +7508,10 @@
     </row>
     <row r="21" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
-        <v>1172</v>
+        <v>1217</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1147</v>
+        <v>1195</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>263</v>
@@ -7484,10 +7553,10 @@
     </row>
     <row r="22" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
-        <v>1173</v>
+        <v>1218</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1148</v>
+        <v>1196</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>268</v>
@@ -7529,10 +7598,10 @@
     </row>
     <row r="23" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="32" t="s">
-        <v>1174</v>
+        <v>1219</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>1149</v>
+        <v>1197</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>274</v>
@@ -7544,7 +7613,7 @@
         <v>276</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>1151</v>
+        <v>1129</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>601</v>
@@ -7574,7 +7643,7 @@
     </row>
     <row r="24" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="32" t="s">
-        <v>1175</v>
+        <v>1220</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>1049</v>
@@ -7589,7 +7658,7 @@
         <v>276</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>1150</v>
+        <v>1128</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>601</v>
@@ -7618,6 +7687,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{6821EB74-DF54-4F98-ACFC-4BD3F7CED1D1}"/>
     <hyperlink ref="F24" r:id="rId2" xr:uid="{1C2E5FA8-591D-4767-9C0D-910A04F94C4B}"/>
@@ -7630,7 +7700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1B755A-BE89-4A69-9C59-9687521C23FC}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
@@ -7652,7 +7722,7 @@
         <v>578</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>1152</v>
+        <v>1130</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>579</v>
@@ -7684,10 +7754,10 @@
     </row>
     <row r="2" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>1176</v>
+        <v>1154</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>1153</v>
+        <v>1131</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>280</v>
@@ -7719,10 +7789,10 @@
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>1177</v>
+        <v>1155</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>1154</v>
+        <v>1132</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>282</v>
@@ -7754,10 +7824,10 @@
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>1178</v>
+        <v>1156</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>1155</v>
+        <v>1133</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>284</v>
@@ -7789,10 +7859,10 @@
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>1179</v>
+        <v>1157</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>1156</v>
+        <v>1134</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>286</v>
@@ -7824,10 +7894,10 @@
     </row>
     <row r="6" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>1180</v>
+        <v>1158</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>1157</v>
+        <v>1135</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>288</v>
@@ -7859,10 +7929,10 @@
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>1181</v>
+        <v>1159</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>1158</v>
+        <v>1136</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>293</v>
@@ -7894,10 +7964,10 @@
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>1182</v>
+        <v>1160</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>1159</v>
+        <v>1137</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>298</v>
@@ -7929,10 +7999,10 @@
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>1183</v>
+        <v>1161</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>1160</v>
+        <v>1138</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>300</v>
@@ -7964,10 +8034,10 @@
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>1184</v>
+        <v>1162</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>1161</v>
+        <v>1139</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>302</v>
@@ -7999,10 +8069,10 @@
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>1185</v>
+        <v>1163</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>1162</v>
+        <v>1140</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>304</v>
@@ -8034,10 +8104,10 @@
     </row>
     <row r="12" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>1186</v>
+        <v>1164</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>1163</v>
+        <v>1141</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>306</v>
@@ -8069,10 +8139,10 @@
     </row>
     <row r="13" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>1187</v>
+        <v>1165</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>1164</v>
+        <v>1142</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>308</v>
@@ -8104,10 +8174,10 @@
     </row>
     <row r="14" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>1188</v>
+        <v>1166</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>1165</v>
+        <v>1143</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>310</v>
@@ -8139,10 +8209,10 @@
     </row>
     <row r="15" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>1189</v>
+        <v>1167</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>1166</v>
+        <v>1144</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>312</v>
@@ -8174,10 +8244,10 @@
     </row>
     <row r="16" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>1190</v>
+        <v>1168</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>1167</v>
+        <v>1145</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>314</v>
@@ -8209,10 +8279,10 @@
     </row>
     <row r="17" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>1191</v>
+        <v>1169</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>1168</v>
+        <v>1146</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>316</v>
@@ -8244,10 +8314,10 @@
     </row>
     <row r="18" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>1192</v>
+        <v>1170</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>1169</v>
+        <v>1147</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>318</v>
@@ -8279,10 +8349,10 @@
     </row>
     <row r="19" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>1193</v>
+        <v>1171</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>1170</v>
+        <v>1148</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>320</v>
@@ -8314,10 +8384,10 @@
     </row>
     <row r="20" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>1194</v>
+        <v>1172</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>1171</v>
+        <v>1149</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>322</v>
@@ -8349,10 +8419,10 @@
     </row>
     <row r="21" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>1195</v>
+        <v>1173</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>1172</v>
+        <v>1150</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>325</v>
@@ -8384,10 +8454,10 @@
     </row>
     <row r="22" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>1196</v>
+        <v>1174</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>1173</v>
+        <v>1151</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>327</v>
@@ -8422,7 +8492,7 @@
         <v>329</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>1174</v>
+        <v>1152</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>330</v>
@@ -8457,7 +8527,7 @@
         <v>1051</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>1175</v>
+        <v>1153</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>330</v>
@@ -8466,7 +8536,7 @@
         <v>331</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>1197</v>
+        <v>1175</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>623</v>

</xml_diff>

<commit_message>
Order List and Details Update
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\BespokeAPI\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AA66C7-AA50-46C1-8633-26C95342F187}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9687A496-F521-41DB-ACCF-CC11FED1550D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="1201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2397" uniqueCount="1203">
   <si>
     <t>CategoryNametext</t>
   </si>
@@ -3641,6 +3641,12 @@
   </si>
   <si>
     <t>option3</t>
+  </si>
+  <si>
+    <t>Delivery Method</t>
+  </si>
+  <si>
+    <t>both</t>
   </si>
 </sst>
 </file>
@@ -3754,7 +3760,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -3792,12 +3798,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3883,6 +3898,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12006,10 +12025,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337AF865-08E8-4C8C-A074-848D6C202917}">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12020,9 +12039,10 @@
     <col min="4" max="4" width="18.140625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>754</v>
       </c>
@@ -12050,8 +12070,11 @@
       <c r="I1" s="35" t="s">
         <v>1196</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="36" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>756</v>
       </c>
@@ -12065,7 +12088,7 @@
         <v>834</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F2" s="8">
         <v>14.25</v>
@@ -12073,14 +12096,15 @@
       <c r="G2" s="8" t="s">
         <v>851</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>1200</v>
-      </c>
+      <c r="H2" s="8"/>
       <c r="I2" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>757</v>
       </c>
@@ -12108,8 +12132,11 @@
       <c r="I3" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>758</v>
       </c>
@@ -12135,8 +12162,11 @@
       <c r="I4" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>759</v>
       </c>
@@ -12162,8 +12192,11 @@
       <c r="I5" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>760</v>
       </c>
@@ -12189,8 +12222,11 @@
       <c r="I6" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>761</v>
       </c>
@@ -12216,8 +12252,11 @@
       <c r="I7" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>762</v>
       </c>
@@ -12245,8 +12284,11 @@
       <c r="I8" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>763</v>
       </c>
@@ -12272,8 +12314,11 @@
       <c r="I9" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>764</v>
       </c>
@@ -12299,8 +12344,11 @@
       <c r="I10" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>765</v>
       </c>
@@ -12326,8 +12374,11 @@
       <c r="I11" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>766</v>
       </c>
@@ -12353,8 +12404,11 @@
       <c r="I12" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>767</v>
       </c>
@@ -12382,8 +12436,11 @@
       <c r="I13" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>768</v>
       </c>
@@ -12409,8 +12466,11 @@
       <c r="I14" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>769</v>
       </c>
@@ -12436,8 +12496,11 @@
       <c r="I15" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>770</v>
       </c>
@@ -12463,8 +12526,11 @@
       <c r="I16" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>771</v>
       </c>
@@ -12490,8 +12556,11 @@
       <c r="I17" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>772</v>
       </c>
@@ -12519,8 +12588,11 @@
       <c r="I18" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>773</v>
       </c>
@@ -12546,8 +12618,11 @@
       <c r="I19" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>774</v>
       </c>
@@ -12573,8 +12648,11 @@
       <c r="I20" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>775</v>
       </c>
@@ -12600,8 +12678,11 @@
       <c r="I21" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>776</v>
       </c>
@@ -12627,8 +12708,11 @@
       <c r="I22" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>777</v>
       </c>
@@ -12656,8 +12740,11 @@
       <c r="I23" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>778</v>
       </c>
@@ -12683,8 +12770,11 @@
       <c r="I24" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>779</v>
       </c>
@@ -12710,8 +12800,11 @@
       <c r="I25" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>780</v>
       </c>
@@ -12737,8 +12830,11 @@
       <c r="I26" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J26" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>781</v>
       </c>
@@ -12764,8 +12860,11 @@
       <c r="I27" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>782</v>
       </c>
@@ -12793,8 +12892,11 @@
       <c r="I28" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>783</v>
       </c>
@@ -12820,8 +12922,11 @@
       <c r="I29" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J29" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>784</v>
       </c>
@@ -12847,8 +12952,11 @@
       <c r="I30" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>785</v>
       </c>
@@ -12874,8 +12982,11 @@
       <c r="I31" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J31" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>786</v>
       </c>
@@ -12901,8 +13012,11 @@
       <c r="I32" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J32" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>787</v>
       </c>
@@ -12930,8 +13044,11 @@
       <c r="I33" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J33" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>788</v>
       </c>
@@ -12957,8 +13074,11 @@
       <c r="I34" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J34" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>789</v>
       </c>
@@ -12984,8 +13104,11 @@
       <c r="I35" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J35" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>790</v>
       </c>
@@ -13011,8 +13134,11 @@
       <c r="I36" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J36" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>791</v>
       </c>
@@ -13038,8 +13164,11 @@
       <c r="I37" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J37" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>792</v>
       </c>
@@ -13067,8 +13196,11 @@
       <c r="I38" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J38" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>793</v>
       </c>
@@ -13094,8 +13226,11 @@
       <c r="I39" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J39" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>794</v>
       </c>
@@ -13121,8 +13256,11 @@
       <c r="I40" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J40" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>795</v>
       </c>
@@ -13148,8 +13286,11 @@
       <c r="I41" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J41" s="37" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>796</v>
       </c>
@@ -13175,8 +13316,11 @@
       <c r="I42" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J42" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>797</v>
       </c>
@@ -13204,8 +13348,11 @@
       <c r="I43" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J43" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>798</v>
       </c>
@@ -13231,8 +13378,11 @@
       <c r="I44" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J44" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>799</v>
       </c>
@@ -13258,8 +13408,11 @@
       <c r="I45" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J45" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>800</v>
       </c>
@@ -13285,8 +13438,11 @@
       <c r="I46" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J46" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>801</v>
       </c>
@@ -13312,8 +13468,11 @@
       <c r="I47" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J47" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>802</v>
       </c>
@@ -13341,8 +13500,11 @@
       <c r="I48" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J48" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>803</v>
       </c>
@@ -13368,8 +13530,11 @@
       <c r="I49" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J49" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>804</v>
       </c>
@@ -13395,8 +13560,11 @@
       <c r="I50" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J50" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>805</v>
       </c>
@@ -13422,8 +13590,11 @@
       <c r="I51" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J51" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>806</v>
       </c>
@@ -13449,8 +13620,11 @@
       <c r="I52" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J52" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>807</v>
       </c>
@@ -13478,8 +13652,11 @@
       <c r="I53" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J53" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>808</v>
       </c>
@@ -13505,8 +13682,11 @@
       <c r="I54" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J54" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>809</v>
       </c>
@@ -13532,8 +13712,11 @@
       <c r="I55" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J55" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>810</v>
       </c>
@@ -13559,8 +13742,11 @@
       <c r="I56" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J56" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>811</v>
       </c>
@@ -13586,8 +13772,11 @@
       <c r="I57" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J57" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>812</v>
       </c>
@@ -13615,8 +13804,11 @@
       <c r="I58" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J58" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>813</v>
       </c>
@@ -13642,8 +13834,11 @@
       <c r="I59" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J59" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>814</v>
       </c>
@@ -13669,8 +13864,11 @@
       <c r="I60" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J60" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>815</v>
       </c>
@@ -13696,8 +13894,11 @@
       <c r="I61" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J61" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>816</v>
       </c>
@@ -13723,8 +13924,11 @@
       <c r="I62" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J62" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>817</v>
       </c>
@@ -13752,8 +13956,11 @@
       <c r="I63" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J63" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>818</v>
       </c>
@@ -13779,8 +13986,11 @@
       <c r="I64" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J64" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>819</v>
       </c>
@@ -13806,8 +14016,11 @@
       <c r="I65" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J65" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>820</v>
       </c>
@@ -13833,8 +14046,11 @@
       <c r="I66" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J66" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>821</v>
       </c>
@@ -13860,8 +14076,11 @@
       <c r="I67" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J67" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>822</v>
       </c>
@@ -13889,8 +14108,11 @@
       <c r="I68" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J68" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>823</v>
       </c>
@@ -13916,8 +14138,11 @@
       <c r="I69" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J69" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>824</v>
       </c>
@@ -13943,8 +14168,11 @@
       <c r="I70" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J70" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>825</v>
       </c>
@@ -13970,8 +14198,11 @@
       <c r="I71" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J71" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>826</v>
       </c>
@@ -13997,8 +14228,11 @@
       <c r="I72" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J72" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>827</v>
       </c>
@@ -14026,8 +14260,11 @@
       <c r="I73" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J73" s="37" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>828</v>
       </c>
@@ -14053,8 +14290,11 @@
       <c r="I74" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J74" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>829</v>
       </c>
@@ -14080,8 +14320,11 @@
       <c r="I75" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J75" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>830</v>
       </c>
@@ -14107,8 +14350,11 @@
       <c r="I76" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J76" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>831</v>
       </c>
@@ -14134,8 +14380,11 @@
       <c r="I77" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J77" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>832</v>
       </c>
@@ -14163,8 +14412,11 @@
       <c r="I78" s="2" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J78" s="37" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>1005</v>
       </c>
@@ -14191,6 +14443,9 @@
       </c>
       <c r="I79" s="2" t="s">
         <v>849</v>
+      </c>
+      <c r="J79" s="37" t="s">
+        <v>1202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Payment & Transaction Complete
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\BespokeAPI\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9687A496-F521-41DB-ACCF-CC11FED1550D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44ECFA7D-949C-41FA-8CE3-B2D196707357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2397" uniqueCount="1203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="1203">
   <si>
     <t>CategoryNametext</t>
   </si>
@@ -2308,12 +2308,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Item01</t>
-  </si>
-  <si>
-    <t>Item02</t>
-  </si>
-  <si>
     <t>Item03</t>
   </si>
   <si>
@@ -3647,6 +3641,12 @@
   </si>
   <si>
     <t>both</t>
+  </si>
+  <si>
+    <t>ItemNoVariants</t>
+  </si>
+  <si>
+    <t>ItemWithVariants</t>
   </si>
 </sst>
 </file>
@@ -6235,7 +6235,7 @@
         <v>741</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>123</v>
@@ -6252,7 +6252,7 @@
         <v>742</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>744</v>
@@ -6269,7 +6269,7 @@
         <v>742</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>744</v>
@@ -6286,7 +6286,7 @@
         <v>742</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>745</v>
@@ -6303,7 +6303,7 @@
         <v>742</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>127</v>
@@ -6320,7 +6320,7 @@
         <v>742</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>744</v>
@@ -6337,7 +6337,7 @@
         <v>742</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>744</v>
@@ -6354,7 +6354,7 @@
         <v>742</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>745</v>
@@ -6371,7 +6371,7 @@
         <v>742</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>127</v>
@@ -6388,7 +6388,7 @@
         <v>742</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>744</v>
@@ -6405,7 +6405,7 @@
         <v>742</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>744</v>
@@ -6422,7 +6422,7 @@
         <v>742</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>745</v>
@@ -6439,7 +6439,7 @@
         <v>742</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>127</v>
@@ -6456,7 +6456,7 @@
         <v>742</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>751</v>
@@ -6538,7 +6538,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>137</v>
@@ -6559,7 +6559,7 @@
         <v>141</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>142</v>
@@ -6585,10 +6585,10 @@
     </row>
     <row r="2" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>148</v>
@@ -6600,7 +6600,7 @@
         <v>150</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>568</v>
@@ -6632,10 +6632,10 @@
     </row>
     <row r="3" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>155</v>
@@ -6647,7 +6647,7 @@
         <v>157</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>576</v>
@@ -6679,10 +6679,10 @@
     </row>
     <row r="4" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>160</v>
@@ -6694,7 +6694,7 @@
         <v>162</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>569</v>
@@ -6724,10 +6724,10 @@
     </row>
     <row r="5" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>165</v>
@@ -6739,7 +6739,7 @@
         <v>167</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>570</v>
@@ -6771,10 +6771,10 @@
     </row>
     <row r="6" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>172</v>
@@ -6786,7 +6786,7 @@
         <v>174</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>571</v>
@@ -6818,10 +6818,10 @@
     </row>
     <row r="7" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>179</v>
@@ -6833,7 +6833,7 @@
         <v>181</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>572</v>
@@ -6865,10 +6865,10 @@
     </row>
     <row r="8" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>185</v>
@@ -6880,7 +6880,7 @@
         <v>187</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>573</v>
@@ -6912,10 +6912,10 @@
     </row>
     <row r="9" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>190</v>
@@ -6927,7 +6927,7 @@
         <v>192</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="G9" s="18" t="s">
         <v>574</v>
@@ -6959,10 +6959,10 @@
     </row>
     <row r="10" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>195</v>
@@ -6974,7 +6974,7 @@
         <v>197</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>575</v>
@@ -7006,10 +7006,10 @@
     </row>
     <row r="11" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>199</v>
@@ -7021,7 +7021,7 @@
         <v>201</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>577</v>
@@ -7053,10 +7053,10 @@
     </row>
     <row r="12" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>204</v>
@@ -7068,7 +7068,7 @@
         <v>206</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="G12" s="18" t="s">
         <v>578</v>
@@ -7100,10 +7100,10 @@
     </row>
     <row r="13" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>209</v>
@@ -7115,7 +7115,7 @@
         <v>211</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="G13" s="18" t="s">
         <v>579</v>
@@ -7147,10 +7147,10 @@
     </row>
     <row r="14" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>214</v>
@@ -7162,7 +7162,7 @@
         <v>216</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>580</v>
@@ -7194,10 +7194,10 @@
     </row>
     <row r="15" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>219</v>
@@ -7209,7 +7209,7 @@
         <v>221</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>581</v>
@@ -7241,10 +7241,10 @@
     </row>
     <row r="16" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>225</v>
@@ -7256,7 +7256,7 @@
         <v>227</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>582</v>
@@ -7288,10 +7288,10 @@
     </row>
     <row r="17" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>230</v>
@@ -7303,7 +7303,7 @@
         <v>232</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>583</v>
@@ -7335,10 +7335,10 @@
     </row>
     <row r="18" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>235</v>
@@ -7350,7 +7350,7 @@
         <v>237</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>584</v>
@@ -7382,10 +7382,10 @@
     </row>
     <row r="19" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>240</v>
@@ -7397,7 +7397,7 @@
         <v>242</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>585</v>
@@ -7427,10 +7427,10 @@
     </row>
     <row r="20" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>244</v>
@@ -7442,7 +7442,7 @@
         <v>246</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>586</v>
@@ -7472,10 +7472,10 @@
     </row>
     <row r="21" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>251</v>
@@ -7487,7 +7487,7 @@
         <v>253</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>587</v>
@@ -7517,10 +7517,10 @@
     </row>
     <row r="22" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>256</v>
@@ -7532,7 +7532,7 @@
         <v>258</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>588</v>
@@ -7562,10 +7562,10 @@
     </row>
     <row r="23" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>262</v>
@@ -7577,7 +7577,7 @@
         <v>264</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>589</v>
@@ -7607,13 +7607,13 @@
     </row>
     <row r="24" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>263</v>
@@ -7622,7 +7622,7 @@
         <v>264</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>589</v>
@@ -7686,7 +7686,7 @@
         <v>566</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>567</v>
@@ -7718,10 +7718,10 @@
     </row>
     <row r="2" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>268</v>
@@ -7730,7 +7730,7 @@
         <v>269</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>590</v>
@@ -7753,10 +7753,10 @@
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>270</v>
@@ -7765,7 +7765,7 @@
         <v>271</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>591</v>
@@ -7788,10 +7788,10 @@
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>272</v>
@@ -7800,7 +7800,7 @@
         <v>273</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>592</v>
@@ -7823,10 +7823,10 @@
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>274</v>
@@ -7835,7 +7835,7 @@
         <v>275</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>593</v>
@@ -7858,10 +7858,10 @@
     </row>
     <row r="6" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>276</v>
@@ -7870,7 +7870,7 @@
         <v>277</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>594</v>
@@ -7893,10 +7893,10 @@
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>281</v>
@@ -7905,7 +7905,7 @@
         <v>282</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>595</v>
@@ -7928,10 +7928,10 @@
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>286</v>
@@ -7940,7 +7940,7 @@
         <v>287</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>596</v>
@@ -7963,10 +7963,10 @@
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>288</v>
@@ -7975,7 +7975,7 @@
         <v>289</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>597</v>
@@ -7998,10 +7998,10 @@
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>290</v>
@@ -8010,7 +8010,7 @@
         <v>291</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>598</v>
@@ -8033,10 +8033,10 @@
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>292</v>
@@ -8045,7 +8045,7 @@
         <v>293</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>599</v>
@@ -8068,10 +8068,10 @@
     </row>
     <row r="12" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>294</v>
@@ -8080,7 +8080,7 @@
         <v>295</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>600</v>
@@ -8103,10 +8103,10 @@
     </row>
     <row r="13" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>296</v>
@@ -8115,7 +8115,7 @@
         <v>297</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>601</v>
@@ -8138,10 +8138,10 @@
     </row>
     <row r="14" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>298</v>
@@ -8150,7 +8150,7 @@
         <v>299</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>602</v>
@@ -8173,10 +8173,10 @@
     </row>
     <row r="15" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>300</v>
@@ -8185,7 +8185,7 @@
         <v>301</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>603</v>
@@ -8208,10 +8208,10 @@
     </row>
     <row r="16" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>302</v>
@@ -8220,7 +8220,7 @@
         <v>303</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>604</v>
@@ -8243,10 +8243,10 @@
     </row>
     <row r="17" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>304</v>
@@ -8255,7 +8255,7 @@
         <v>305</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>605</v>
@@ -8278,10 +8278,10 @@
     </row>
     <row r="18" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>306</v>
@@ -8290,7 +8290,7 @@
         <v>307</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>606</v>
@@ -8313,10 +8313,10 @@
     </row>
     <row r="19" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>308</v>
@@ -8325,7 +8325,7 @@
         <v>309</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>607</v>
@@ -8348,10 +8348,10 @@
     </row>
     <row r="20" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>310</v>
@@ -8360,7 +8360,7 @@
         <v>311</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="F20" s="18" t="s">
         <v>608</v>
@@ -8383,10 +8383,10 @@
     </row>
     <row r="21" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>313</v>
@@ -8395,7 +8395,7 @@
         <v>314</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>609</v>
@@ -8418,10 +8418,10 @@
     </row>
     <row r="22" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>315</v>
@@ -8430,7 +8430,7 @@
         <v>316</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="F22" s="18" t="s">
         <v>610</v>
@@ -8456,7 +8456,7 @@
         <v>317</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>318</v>
@@ -8465,7 +8465,7 @@
         <v>319</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="F23" s="18" t="s">
         <v>611</v>
@@ -8488,10 +8488,10 @@
     </row>
     <row r="24" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>318</v>
@@ -8500,7 +8500,7 @@
         <v>319</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>611</v>
@@ -11804,7 +11804,7 @@
         <v>322</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -12028,12 +12028,12 @@
   <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="76.140625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1" collapsed="1"/>
@@ -12050,55 +12050,55 @@
         <v>755</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>752</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>756</v>
+        <v>1201</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C2" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F2" s="8">
         <v>14.25</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="H2" s="8"/>
-      <c r="I2" s="2" t="s">
-        <v>849</v>
+      <c r="I2" s="2">
+        <v>6</v>
       </c>
       <c r="J2" s="37" t="s">
         <v>742</v>
@@ -12106,31 +12106,31 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>757</v>
+        <v>1202</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C3" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F3" s="2">
         <v>10.25</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>1198</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>849</v>
+        <v>1196</v>
+      </c>
+      <c r="I3" s="2">
+        <v>6</v>
       </c>
       <c r="J3" s="37" t="s">
         <v>742</v>
@@ -12138,29 +12138,29 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C4" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F4" s="8">
         <v>14</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J4" s="37" t="s">
         <v>742</v>
@@ -12168,29 +12168,29 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C5" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F5" s="8">
         <v>17</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J5" s="37" t="s">
         <v>742</v>
@@ -12198,29 +12198,29 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C6" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F6" s="8">
         <v>14.25</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J6" s="37" t="s">
         <v>742</v>
@@ -12228,29 +12228,29 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C7" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F7" s="8">
         <v>14.25</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J7" s="37" t="s">
         <v>742</v>
@@ -12258,31 +12258,31 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C8" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F8" s="2">
         <v>10.25</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J8" s="37" t="s">
         <v>742</v>
@@ -12290,29 +12290,29 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C9" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F9" s="8">
         <v>14</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J9" s="37" t="s">
         <v>742</v>
@@ -12320,29 +12320,29 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C10" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F10" s="8">
         <v>17</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J10" s="37" t="s">
         <v>742</v>
@@ -12350,29 +12350,29 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C11" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>631</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F11" s="8">
         <v>14.25</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J11" s="37" t="s">
         <v>742</v>
@@ -12380,29 +12380,29 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C12" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>632</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F12" s="8">
         <v>14.25</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J12" s="37" t="s">
         <v>742</v>
@@ -12410,31 +12410,31 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C13" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>633</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F13" s="2">
         <v>10.25</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J13" s="37" t="s">
         <v>742</v>
@@ -12442,29 +12442,29 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C14" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>634</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F14" s="8">
         <v>14</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J14" s="37" t="s">
         <v>742</v>
@@ -12472,29 +12472,29 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C15" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>635</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F15" s="8">
         <v>17</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J15" s="37" t="s">
         <v>742</v>
@@ -12502,29 +12502,29 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C16" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>636</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F16" s="8">
         <v>14.25</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J16" s="37" t="s">
         <v>742</v>
@@ -12532,29 +12532,29 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C17" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>637</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F17" s="8">
         <v>14.25</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J17" s="37" t="s">
         <v>742</v>
@@ -12562,31 +12562,31 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C18" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>638</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F18" s="2">
         <v>10.25</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J18" s="37" t="s">
         <v>742</v>
@@ -12594,29 +12594,29 @@
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C19" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>639</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F19" s="8">
         <v>14</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J19" s="37" t="s">
         <v>742</v>
@@ -12624,25 +12624,25 @@
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C20" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>640</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F20" s="8">
         <v>17</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8">
@@ -12654,59 +12654,59 @@
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C21" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>641</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F21" s="8">
         <v>14.25</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8">
         <v>1000</v>
       </c>
       <c r="J21" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C22" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>642</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F22" s="8">
         <v>14.25</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J22" s="37" t="s">
         <v>742</v>
@@ -12714,61 +12714,61 @@
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C23" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>643</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F23" s="2">
         <v>10.25</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="I23" s="8">
         <v>1000</v>
       </c>
       <c r="J23" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C24" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>644</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F24" s="8">
         <v>14</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J24" s="37" t="s">
         <v>742</v>
@@ -12776,25 +12776,25 @@
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C25" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>645</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F25" s="8">
         <v>17</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="8">
@@ -12806,59 +12806,59 @@
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C26" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>646</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F26" s="8">
         <v>14.25</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="8">
         <v>1000</v>
       </c>
       <c r="J26" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C27" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>647</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F27" s="8">
         <v>14.25</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J27" s="37" t="s">
         <v>742</v>
@@ -12866,61 +12866,61 @@
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C28" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>648</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F28" s="2">
         <v>10.25</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="I28" s="8">
         <v>1000</v>
       </c>
       <c r="J28" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C29" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>649</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F29" s="8">
         <v>14</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J29" s="37" t="s">
         <v>742</v>
@@ -12928,25 +12928,25 @@
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C30" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>650</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F30" s="8">
         <v>17</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="8">
@@ -12958,59 +12958,59 @@
     </row>
     <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C31" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>651</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F31" s="8">
         <v>14.25</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="8">
         <v>1000</v>
       </c>
       <c r="J31" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C32" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>652</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F32" s="8">
         <v>14.25</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J32" s="37" t="s">
         <v>742</v>
@@ -13018,61 +13018,61 @@
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C33" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>653</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F33" s="2">
         <v>10.25</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="I33" s="8">
         <v>1000</v>
       </c>
       <c r="J33" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C34" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>654</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F34" s="8">
         <v>14</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J34" s="37" t="s">
         <v>742</v>
@@ -13080,25 +13080,25 @@
     </row>
     <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C35" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>655</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F35" s="8">
         <v>17</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="H35" s="8"/>
       <c r="I35" s="8">
@@ -13110,59 +13110,59 @@
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C36" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>656</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F36" s="8">
         <v>14.25</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="H36" s="8"/>
       <c r="I36" s="8">
         <v>1000</v>
       </c>
       <c r="J36" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C37" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>657</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F37" s="8">
         <v>14.25</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="H37" s="8"/>
       <c r="I37" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J37" s="37" t="s">
         <v>742</v>
@@ -13170,28 +13170,28 @@
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C38" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>658</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F38" s="2">
         <v>10.25</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="I38" s="2">
         <v>0</v>
@@ -13202,25 +13202,25 @@
     </row>
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C39" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>659</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F39" s="8">
         <v>14</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="H39" s="8"/>
       <c r="I39" s="2">
@@ -13232,25 +13232,25 @@
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C40" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>660</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F40" s="8">
         <v>17</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="H40" s="8"/>
       <c r="I40" s="2">
@@ -13262,25 +13262,25 @@
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C41" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>661</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F41" s="8">
         <v>14.25</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="H41" s="8"/>
       <c r="I41" s="2">
@@ -13292,58 +13292,58 @@
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C42" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>662</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F42" s="8">
         <v>14.25</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="H42" s="8"/>
       <c r="I42" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J42" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C43" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>663</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F43" s="2">
         <v>10.25</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="I43" s="2">
         <v>0</v>
@@ -13354,55 +13354,55 @@
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C44" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>664</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F44" s="8">
         <v>14</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J44" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C45" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>665</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F45" s="8">
         <v>17</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="H45" s="8"/>
       <c r="I45" s="2">
@@ -13414,25 +13414,25 @@
     </row>
     <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C46" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>666</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F46" s="8">
         <v>14.25</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="H46" s="8"/>
       <c r="I46" s="2">
@@ -13444,58 +13444,58 @@
     </row>
     <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C47" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>667</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F47" s="8">
         <v>14.25</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="H47" s="8"/>
       <c r="I47" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J47" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C48" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>668</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F48" s="2">
         <v>10.25</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="I48" s="2">
         <v>0</v>
@@ -13506,55 +13506,55 @@
     </row>
     <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C49" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>669</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F49" s="8">
         <v>14</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="H49" s="8"/>
       <c r="I49" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J49" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C50" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>670</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F50" s="8">
         <v>17</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="H50" s="8"/>
       <c r="I50" s="2">
@@ -13566,25 +13566,25 @@
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C51" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>671</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F51" s="8">
         <v>14.25</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="H51" s="8"/>
       <c r="I51" s="2">
@@ -13596,58 +13596,58 @@
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C52" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>672</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F52" s="8">
         <v>14.25</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="H52" s="8"/>
       <c r="I52" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J52" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C53" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>673</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F53" s="2">
         <v>10.25</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="I53" s="2">
         <v>0</v>
@@ -13658,55 +13658,55 @@
     </row>
     <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C54" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>674</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F54" s="8">
         <v>14</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J54" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C55" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>675</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F55" s="8">
         <v>17</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H55" s="8"/>
       <c r="I55" s="2">
@@ -13718,88 +13718,88 @@
     </row>
     <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C56" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>676</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F56" s="8">
         <v>14.25</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="H56" s="8"/>
       <c r="I56" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J56" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C57" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>677</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F57" s="8">
         <v>14.25</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="H57" s="8"/>
       <c r="I57" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J57" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C58" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>678</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F58" s="2">
         <v>10.25</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="I58" s="2">
         <v>0</v>
@@ -13810,148 +13810,148 @@
     </row>
     <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C59" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>679</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F59" s="8">
         <v>14</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="H59" s="8"/>
       <c r="I59" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J59" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C60" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>680</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F60" s="8">
         <v>17</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="H60" s="8"/>
       <c r="I60" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J60" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C61" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>681</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F61" s="8">
         <v>14.25</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="H61" s="8"/>
       <c r="I61" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J61" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C62" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>682</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F62" s="8">
         <v>14.25</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="H62" s="8"/>
       <c r="I62" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J62" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C63" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>683</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F63" s="2">
         <v>10.25</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="I63" s="2">
         <v>0</v>
@@ -13962,148 +13962,148 @@
     </row>
     <row r="64" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C64" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>684</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F64" s="8">
         <v>14</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="H64" s="8"/>
       <c r="I64" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J64" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C65" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>685</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F65" s="8">
         <v>17</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="H65" s="8"/>
       <c r="I65" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J65" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C66" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>686</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F66" s="8">
         <v>14.25</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="H66" s="8"/>
       <c r="I66" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J66" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C67" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>687</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F67" s="8">
         <v>14.25</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="H67" s="8"/>
       <c r="I67" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J67" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C68" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>688</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F68" s="2">
         <v>10.25</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="I68" s="2">
         <v>0</v>
@@ -14114,148 +14114,148 @@
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C69" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>689</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F69" s="8">
         <v>14</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="H69" s="8"/>
       <c r="I69" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J69" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C70" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>690</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F70" s="8">
         <v>17</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="H70" s="8"/>
       <c r="I70" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J70" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C71" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>691</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F71" s="8">
         <v>14.25</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="H71" s="8"/>
       <c r="I71" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J71" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C72" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>692</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F72" s="8">
         <v>14.25</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="H72" s="8"/>
       <c r="I72" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J72" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C73" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>693</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F73" s="2">
         <v>10.25</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="I73" s="2">
         <v>0</v>
@@ -14266,186 +14266,186 @@
     </row>
     <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C74" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>694</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F74" s="8">
         <v>15</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="H74" s="8"/>
       <c r="I74" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J74" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C75" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>695</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F75" s="8">
         <v>15</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="H75" s="8"/>
       <c r="I75" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J75" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C76" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>696</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F76" s="8">
         <v>15</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="H76" s="8"/>
       <c r="I76" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J76" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C77" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>697</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F77" s="8">
         <v>15</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="H77" s="8"/>
       <c r="I77" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="J77" s="37" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>698</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F78" s="8">
         <v>15</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="H78" s="8" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="J78" s="37" t="s">
         <v>1200</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>849</v>
-      </c>
-      <c r="J78" s="37" t="s">
-        <v>1202</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C79" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F79" s="8">
         <v>15</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="H79" s="8" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="J79" s="37" t="s">
         <v>1200</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>849</v>
-      </c>
-      <c r="J79" s="37" t="s">
-        <v>1202</v>
       </c>
     </row>
   </sheetData>
@@ -14488,111 +14488,111 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C1" t="s">
         <v>1011</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1012</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>1013</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>1014</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>1015</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1016</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1017</v>
       </c>
       <c r="H1" t="s">
         <v>123</v>
       </c>
       <c r="I1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="K1" t="s">
         <v>1018</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>1019</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>1020</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1021</v>
-      </c>
-      <c r="M1" t="s">
-        <v>1022</v>
       </c>
       <c r="N1" t="s">
         <v>731</v>
       </c>
       <c r="O1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="Q1" t="s">
         <v>1023</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>1024</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>1025</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>1026</v>
-      </c>
-      <c r="S1" t="s">
-        <v>1027</v>
-      </c>
-      <c r="T1" t="s">
-        <v>1028</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C2" t="s">
         <v>1029</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H2" t="s">
         <v>1030</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2" t="s">
         <v>1031</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>1032</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" s="28" t="s">
+        <v>1038</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="M2" t="s">
         <v>1033</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>1034</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="O2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="P2" t="s">
         <v>1040</v>
       </c>
-      <c r="L2" t="s">
-        <v>1031</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>1035</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>1036</v>
       </c>
-      <c r="O2" t="s">
-        <v>1041</v>
-      </c>
-      <c r="P2" t="s">
-        <v>1042</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>1037</v>
-      </c>
-      <c r="R2" t="s">
-        <v>1038</v>
-      </c>
-      <c r="S2" t="s">
-        <v>1039</v>
       </c>
       <c r="T2">
         <v>20</v>

</xml_diff>

<commit_message>
Update Add Item (Data Application)
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\BespokeAPI\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44ECFA7D-949C-41FA-8CE3-B2D196707357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB53713B-8491-4750-8D03-D6C5CC0BF1BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{6DADBD4C-F1D0-4CA8-9C8D-D312492A8BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin Category" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="1203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="1065">
   <si>
     <t>CategoryNametext</t>
   </si>
@@ -2308,231 +2308,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Item03</t>
-  </si>
-  <si>
-    <t>Item04</t>
-  </si>
-  <si>
-    <t>Item05</t>
-  </si>
-  <si>
-    <t>Item06</t>
-  </si>
-  <si>
-    <t>Item07</t>
-  </si>
-  <si>
-    <t>Item08</t>
-  </si>
-  <si>
-    <t>Item09</t>
-  </si>
-  <si>
-    <t>Item10</t>
-  </si>
-  <si>
-    <t>Item11</t>
-  </si>
-  <si>
-    <t>Item12</t>
-  </si>
-  <si>
-    <t>Item13</t>
-  </si>
-  <si>
-    <t>Item14</t>
-  </si>
-  <si>
-    <t>Item15</t>
-  </si>
-  <si>
-    <t>Item16</t>
-  </si>
-  <si>
-    <t>Item17</t>
-  </si>
-  <si>
-    <t>Item18</t>
-  </si>
-  <si>
-    <t>Item19</t>
-  </si>
-  <si>
-    <t>Item20</t>
-  </si>
-  <si>
-    <t>Item21</t>
-  </si>
-  <si>
-    <t>Item22</t>
-  </si>
-  <si>
-    <t>Item23</t>
-  </si>
-  <si>
-    <t>Item24</t>
-  </si>
-  <si>
-    <t>Item25</t>
-  </si>
-  <si>
-    <t>Item26</t>
-  </si>
-  <si>
-    <t>Item27</t>
-  </si>
-  <si>
-    <t>Item28</t>
-  </si>
-  <si>
-    <t>Item29</t>
-  </si>
-  <si>
-    <t>Item30</t>
-  </si>
-  <si>
-    <t>Item31</t>
-  </si>
-  <si>
-    <t>Item32</t>
-  </si>
-  <si>
-    <t>Item33</t>
-  </si>
-  <si>
-    <t>Item34</t>
-  </si>
-  <si>
-    <t>Item35</t>
-  </si>
-  <si>
-    <t>Item36</t>
-  </si>
-  <si>
-    <t>Item37</t>
-  </si>
-  <si>
-    <t>Item38</t>
-  </si>
-  <si>
-    <t>Item39</t>
-  </si>
-  <si>
-    <t>Item40</t>
-  </si>
-  <si>
-    <t>Item41</t>
-  </si>
-  <si>
-    <t>Item42</t>
-  </si>
-  <si>
-    <t>Item43</t>
-  </si>
-  <si>
-    <t>Item44</t>
-  </si>
-  <si>
-    <t>Item45</t>
-  </si>
-  <si>
-    <t>Item46</t>
-  </si>
-  <si>
-    <t>Item47</t>
-  </si>
-  <si>
-    <t>Item48</t>
-  </si>
-  <si>
-    <t>Item49</t>
-  </si>
-  <si>
-    <t>Item50</t>
-  </si>
-  <si>
-    <t>Item51</t>
-  </si>
-  <si>
-    <t>Item52</t>
-  </si>
-  <si>
-    <t>Item53</t>
-  </si>
-  <si>
-    <t>Item54</t>
-  </si>
-  <si>
-    <t>Item55</t>
-  </si>
-  <si>
-    <t>Item56</t>
-  </si>
-  <si>
-    <t>Item57</t>
-  </si>
-  <si>
-    <t>Item58</t>
-  </si>
-  <si>
-    <t>Item59</t>
-  </si>
-  <si>
-    <t>Item60</t>
-  </si>
-  <si>
-    <t>Item61</t>
-  </si>
-  <si>
-    <t>Item62</t>
-  </si>
-  <si>
-    <t>Item63</t>
-  </si>
-  <si>
-    <t>Item64</t>
-  </si>
-  <si>
-    <t>Item65</t>
-  </si>
-  <si>
-    <t>Item66</t>
-  </si>
-  <si>
-    <t>Item67</t>
-  </si>
-  <si>
-    <t>Item68</t>
-  </si>
-  <si>
-    <t>Item69</t>
-  </si>
-  <si>
-    <t>Item70</t>
-  </si>
-  <si>
-    <t>Item71</t>
-  </si>
-  <si>
-    <t>Item72</t>
-  </si>
-  <si>
-    <t>Item73</t>
-  </si>
-  <si>
-    <t>Item74</t>
-  </si>
-  <si>
-    <t>Item75</t>
-  </si>
-  <si>
-    <t>Item76</t>
-  </si>
-  <si>
-    <t>Item77</t>
-  </si>
-  <si>
     <t>ItemImage</t>
   </si>
   <si>
@@ -2677,144 +2452,6 @@
     <t>SKU030</t>
   </si>
   <si>
-    <t>SKU031</t>
-  </si>
-  <si>
-    <t>SKU032</t>
-  </si>
-  <si>
-    <t>SKU033</t>
-  </si>
-  <si>
-    <t>SKU034</t>
-  </si>
-  <si>
-    <t>SKU035</t>
-  </si>
-  <si>
-    <t>SKU036</t>
-  </si>
-  <si>
-    <t>SKU037</t>
-  </si>
-  <si>
-    <t>SKU038</t>
-  </si>
-  <si>
-    <t>SKU039</t>
-  </si>
-  <si>
-    <t>SKU040</t>
-  </si>
-  <si>
-    <t>SKU041</t>
-  </si>
-  <si>
-    <t>SKU042</t>
-  </si>
-  <si>
-    <t>SKU043</t>
-  </si>
-  <si>
-    <t>SKU044</t>
-  </si>
-  <si>
-    <t>SKU045</t>
-  </si>
-  <si>
-    <t>SKU046</t>
-  </si>
-  <si>
-    <t>SKU047</t>
-  </si>
-  <si>
-    <t>SKU048</t>
-  </si>
-  <si>
-    <t>SKU049</t>
-  </si>
-  <si>
-    <t>SKU050</t>
-  </si>
-  <si>
-    <t>SKU051</t>
-  </si>
-  <si>
-    <t>SKU052</t>
-  </si>
-  <si>
-    <t>SKU053</t>
-  </si>
-  <si>
-    <t>SKU054</t>
-  </si>
-  <si>
-    <t>SKU055</t>
-  </si>
-  <si>
-    <t>SKU056</t>
-  </si>
-  <si>
-    <t>SKU057</t>
-  </si>
-  <si>
-    <t>SKU058</t>
-  </si>
-  <si>
-    <t>SKU059</t>
-  </si>
-  <si>
-    <t>SKU060</t>
-  </si>
-  <si>
-    <t>SKU061</t>
-  </si>
-  <si>
-    <t>SKU062</t>
-  </si>
-  <si>
-    <t>SKU063</t>
-  </si>
-  <si>
-    <t>SKU064</t>
-  </si>
-  <si>
-    <t>SKU065</t>
-  </si>
-  <si>
-    <t>SKU066</t>
-  </si>
-  <si>
-    <t>SKU067</t>
-  </si>
-  <si>
-    <t>SKU068</t>
-  </si>
-  <si>
-    <t>SKU069</t>
-  </si>
-  <si>
-    <t>SKU070</t>
-  </si>
-  <si>
-    <t>SKU071</t>
-  </si>
-  <si>
-    <t>SKU072</t>
-  </si>
-  <si>
-    <t>SKU073</t>
-  </si>
-  <si>
-    <t>SKU074</t>
-  </si>
-  <si>
-    <t>SKU075</t>
-  </si>
-  <si>
-    <t>SKU076</t>
-  </si>
-  <si>
     <t>SKU077</t>
   </si>
   <si>
@@ -2917,144 +2554,9 @@
     <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item32.jpg</t>
   </si>
   <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item33.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item34.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item35.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item36.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item37.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item38.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item39.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item40.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item41.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item42.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item43.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item45.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item46.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item47.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item48.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item49.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item50.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item51.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item52.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item53.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item54.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item55.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item56.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item57.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item58.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item59.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item60.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item61.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item62.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item63.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item64.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item65.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item66.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item67.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item68.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item69.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item70.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item71.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item72.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item73.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item74.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item75.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item76.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item77.jpg</t>
-  </si>
-  <si>
     <t>ITEM FOR EDIT</t>
   </si>
   <si>
-    <t>C:\\Users\\Arcadier\\git\\Trillia\\Images\\UN Items\\item78.jpg</t>
-  </si>
-  <si>
     <t>SKU078</t>
   </si>
   <si>
@@ -3625,28 +3127,112 @@
     <t>Stock</t>
   </si>
   <si>
-    <t>Variant Option</t>
-  </si>
-  <si>
-    <t>option1</t>
-  </si>
-  <si>
-    <t>option2</t>
-  </si>
-  <si>
-    <t>option3</t>
-  </si>
-  <si>
     <t>Delivery Method</t>
   </si>
   <si>
     <t>both</t>
   </si>
   <si>
-    <t>ItemNoVariants</t>
-  </si>
-  <si>
-    <t>ItemWithVariants</t>
+    <t>Item_01</t>
+  </si>
+  <si>
+    <t>Item_02</t>
+  </si>
+  <si>
+    <t>Item_03</t>
+  </si>
+  <si>
+    <t>Item_04</t>
+  </si>
+  <si>
+    <t>Item_05</t>
+  </si>
+  <si>
+    <t>Item_06</t>
+  </si>
+  <si>
+    <t>Item_07</t>
+  </si>
+  <si>
+    <t>Item_08</t>
+  </si>
+  <si>
+    <t>Item_09</t>
+  </si>
+  <si>
+    <t>Item_10</t>
+  </si>
+  <si>
+    <t>Item_11</t>
+  </si>
+  <si>
+    <t>Item_12</t>
+  </si>
+  <si>
+    <t>Item_13</t>
+  </si>
+  <si>
+    <t>Item_14</t>
+  </si>
+  <si>
+    <t>Item_15</t>
+  </si>
+  <si>
+    <t>Item_16</t>
+  </si>
+  <si>
+    <t>Item_17</t>
+  </si>
+  <si>
+    <t>Item_18</t>
+  </si>
+  <si>
+    <t>Item_19</t>
+  </si>
+  <si>
+    <t>Item_20</t>
+  </si>
+  <si>
+    <t>Item_21</t>
+  </si>
+  <si>
+    <t>Item_22</t>
+  </si>
+  <si>
+    <t>Item_23</t>
+  </si>
+  <si>
+    <t>Item_24</t>
+  </si>
+  <si>
+    <t>Item_25</t>
+  </si>
+  <si>
+    <t>Item_26</t>
+  </si>
+  <si>
+    <t>Item_27</t>
+  </si>
+  <si>
+    <t>Item_28</t>
+  </si>
+  <si>
+    <t>Item_29</t>
+  </si>
+  <si>
+    <t>Item_30</t>
+  </si>
+  <si>
+    <t>Item_31</t>
+  </si>
+  <si>
+    <t>Variant Image</t>
+  </si>
+  <si>
+    <t>with image</t>
+  </si>
+  <si>
+    <t>without image</t>
   </si>
 </sst>
 </file>
@@ -6235,7 +5821,7 @@
         <v>741</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>1191</v>
+        <v>1025</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>123</v>
@@ -6252,7 +5838,7 @@
         <v>742</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>1178</v>
+        <v>1012</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>744</v>
@@ -6269,7 +5855,7 @@
         <v>742</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>1179</v>
+        <v>1013</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>744</v>
@@ -6286,7 +5872,7 @@
         <v>742</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>1180</v>
+        <v>1014</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>745</v>
@@ -6303,7 +5889,7 @@
         <v>742</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>1181</v>
+        <v>1015</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>127</v>
@@ -6320,7 +5906,7 @@
         <v>742</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>1182</v>
+        <v>1016</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>744</v>
@@ -6337,7 +5923,7 @@
         <v>742</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>1183</v>
+        <v>1017</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>744</v>
@@ -6354,7 +5940,7 @@
         <v>742</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>1184</v>
+        <v>1018</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>745</v>
@@ -6371,7 +5957,7 @@
         <v>742</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>1185</v>
+        <v>1019</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>127</v>
@@ -6388,7 +5974,7 @@
         <v>742</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>1186</v>
+        <v>1020</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>744</v>
@@ -6405,7 +5991,7 @@
         <v>742</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>1187</v>
+        <v>1021</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>744</v>
@@ -6422,7 +6008,7 @@
         <v>742</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>1188</v>
+        <v>1022</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>745</v>
@@ -6439,7 +6025,7 @@
         <v>742</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>1189</v>
+        <v>1023</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>127</v>
@@ -6456,7 +6042,7 @@
         <v>742</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>1190</v>
+        <v>1024</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>751</v>
@@ -6538,7 +6124,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>1087</v>
+        <v>921</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>137</v>
@@ -6559,7 +6145,7 @@
         <v>141</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>1084</v>
+        <v>918</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>142</v>
@@ -6585,10 +6171,10 @@
     </row>
     <row r="2" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>1155</v>
+        <v>989</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1133</v>
+        <v>967</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>148</v>
@@ -6600,7 +6186,7 @@
         <v>150</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1041</v>
+        <v>875</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>568</v>
@@ -6632,10 +6218,10 @@
     </row>
     <row r="3" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
-        <v>1156</v>
+        <v>990</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1134</v>
+        <v>968</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>155</v>
@@ -6647,7 +6233,7 @@
         <v>157</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1042</v>
+        <v>876</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>576</v>
@@ -6679,10 +6265,10 @@
     </row>
     <row r="4" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
-        <v>1157</v>
+        <v>991</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1135</v>
+        <v>969</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>160</v>
@@ -6694,7 +6280,7 @@
         <v>162</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>1043</v>
+        <v>877</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>569</v>
@@ -6724,10 +6310,10 @@
     </row>
     <row r="5" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
-        <v>1158</v>
+        <v>992</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1136</v>
+        <v>970</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>165</v>
@@ -6739,7 +6325,7 @@
         <v>167</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>1044</v>
+        <v>878</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>570</v>
@@ -6771,10 +6357,10 @@
     </row>
     <row r="6" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
-        <v>1159</v>
+        <v>993</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1137</v>
+        <v>971</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>172</v>
@@ -6786,7 +6372,7 @@
         <v>174</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>1045</v>
+        <v>879</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>571</v>
@@ -6818,10 +6404,10 @@
     </row>
     <row r="7" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
-        <v>1160</v>
+        <v>994</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1138</v>
+        <v>972</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>179</v>
@@ -6833,7 +6419,7 @@
         <v>181</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>1046</v>
+        <v>880</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>572</v>
@@ -6865,10 +6451,10 @@
     </row>
     <row r="8" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
-        <v>1161</v>
+        <v>995</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1139</v>
+        <v>973</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>185</v>
@@ -6880,7 +6466,7 @@
         <v>187</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>1047</v>
+        <v>881</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>573</v>
@@ -6912,10 +6498,10 @@
     </row>
     <row r="9" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
-        <v>1162</v>
+        <v>996</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1140</v>
+        <v>974</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>190</v>
@@ -6927,7 +6513,7 @@
         <v>192</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>1048</v>
+        <v>882</v>
       </c>
       <c r="G9" s="18" t="s">
         <v>574</v>
@@ -6959,10 +6545,10 @@
     </row>
     <row r="10" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
-        <v>1163</v>
+        <v>997</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1141</v>
+        <v>975</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>195</v>
@@ -6974,7 +6560,7 @@
         <v>197</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>1049</v>
+        <v>883</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>575</v>
@@ -7006,10 +6592,10 @@
     </row>
     <row r="11" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
-        <v>1164</v>
+        <v>998</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1142</v>
+        <v>976</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>199</v>
@@ -7021,7 +6607,7 @@
         <v>201</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>1050</v>
+        <v>884</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>577</v>
@@ -7053,10 +6639,10 @@
     </row>
     <row r="12" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>1165</v>
+        <v>999</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1143</v>
+        <v>977</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>204</v>
@@ -7068,7 +6654,7 @@
         <v>206</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>1051</v>
+        <v>885</v>
       </c>
       <c r="G12" s="18" t="s">
         <v>578</v>
@@ -7100,10 +6686,10 @@
     </row>
     <row r="13" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
-        <v>1166</v>
+        <v>1000</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1144</v>
+        <v>978</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>209</v>
@@ -7115,7 +6701,7 @@
         <v>211</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>1052</v>
+        <v>886</v>
       </c>
       <c r="G13" s="18" t="s">
         <v>579</v>
@@ -7147,10 +6733,10 @@
     </row>
     <row r="14" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
-        <v>1167</v>
+        <v>1001</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1145</v>
+        <v>979</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>214</v>
@@ -7162,7 +6748,7 @@
         <v>216</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>1053</v>
+        <v>887</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>580</v>
@@ -7194,10 +6780,10 @@
     </row>
     <row r="15" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>1168</v>
+        <v>1002</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1146</v>
+        <v>980</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>219</v>
@@ -7209,7 +6795,7 @@
         <v>221</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>1054</v>
+        <v>888</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>581</v>
@@ -7241,10 +6827,10 @@
     </row>
     <row r="16" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
-        <v>1169</v>
+        <v>1003</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1147</v>
+        <v>981</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>225</v>
@@ -7256,7 +6842,7 @@
         <v>227</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>1055</v>
+        <v>889</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>582</v>
@@ -7288,10 +6874,10 @@
     </row>
     <row r="17" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
-        <v>1170</v>
+        <v>1004</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>1148</v>
+        <v>982</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>230</v>
@@ -7303,7 +6889,7 @@
         <v>232</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>1056</v>
+        <v>890</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>583</v>
@@ -7335,10 +6921,10 @@
     </row>
     <row r="18" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
-        <v>1171</v>
+        <v>1005</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1149</v>
+        <v>983</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>235</v>
@@ -7350,7 +6936,7 @@
         <v>237</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>1057</v>
+        <v>891</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>584</v>
@@ -7382,10 +6968,10 @@
     </row>
     <row r="19" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
-        <v>1172</v>
+        <v>1006</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1150</v>
+        <v>984</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>240</v>
@@ -7397,7 +6983,7 @@
         <v>242</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>1058</v>
+        <v>892</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>585</v>
@@ -7427,10 +7013,10 @@
     </row>
     <row r="20" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
-        <v>1173</v>
+        <v>1007</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>1151</v>
+        <v>985</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>244</v>
@@ -7442,7 +7028,7 @@
         <v>246</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>1059</v>
+        <v>893</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>586</v>
@@ -7472,10 +7058,10 @@
     </row>
     <row r="21" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>1174</v>
+        <v>1008</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1152</v>
+        <v>986</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>251</v>
@@ -7487,7 +7073,7 @@
         <v>253</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>1060</v>
+        <v>894</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>587</v>
@@ -7517,10 +7103,10 @@
     </row>
     <row r="22" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>1175</v>
+        <v>1009</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1153</v>
+        <v>987</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>256</v>
@@ -7532,7 +7118,7 @@
         <v>258</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>1061</v>
+        <v>895</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>588</v>
@@ -7562,10 +7148,10 @@
     </row>
     <row r="23" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
-        <v>1176</v>
+        <v>1010</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>1154</v>
+        <v>988</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>262</v>
@@ -7577,7 +7163,7 @@
         <v>264</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>1086</v>
+        <v>920</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>589</v>
@@ -7607,13 +7193,13 @@
     </row>
     <row r="24" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
-        <v>1177</v>
+        <v>1011</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>1006</v>
+        <v>840</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>1007</v>
+        <v>841</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>263</v>
@@ -7622,7 +7208,7 @@
         <v>264</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>1085</v>
+        <v>919</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>589</v>
@@ -7686,7 +7272,7 @@
         <v>566</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>1087</v>
+        <v>921</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>567</v>
@@ -7718,10 +7304,10 @@
     </row>
     <row r="2" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>1111</v>
+        <v>945</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>1088</v>
+        <v>922</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>268</v>
@@ -7730,7 +7316,7 @@
         <v>269</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>1062</v>
+        <v>896</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>590</v>
@@ -7753,10 +7339,10 @@
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>1112</v>
+        <v>946</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>1089</v>
+        <v>923</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>270</v>
@@ -7765,7 +7351,7 @@
         <v>271</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>1063</v>
+        <v>897</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>591</v>
@@ -7788,10 +7374,10 @@
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>1113</v>
+        <v>947</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>1090</v>
+        <v>924</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>272</v>
@@ -7800,7 +7386,7 @@
         <v>273</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>1064</v>
+        <v>898</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>592</v>
@@ -7823,10 +7409,10 @@
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>1114</v>
+        <v>948</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>1091</v>
+        <v>925</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>274</v>
@@ -7835,7 +7421,7 @@
         <v>275</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>1065</v>
+        <v>899</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>593</v>
@@ -7858,10 +7444,10 @@
     </row>
     <row r="6" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>1115</v>
+        <v>949</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>1092</v>
+        <v>926</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>276</v>
@@ -7870,7 +7456,7 @@
         <v>277</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>1066</v>
+        <v>900</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>594</v>
@@ -7893,10 +7479,10 @@
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>1116</v>
+        <v>950</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>1093</v>
+        <v>927</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>281</v>
@@ -7905,7 +7491,7 @@
         <v>282</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>1067</v>
+        <v>901</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>595</v>
@@ -7928,10 +7514,10 @@
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>1117</v>
+        <v>951</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>1094</v>
+        <v>928</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>286</v>
@@ -7940,7 +7526,7 @@
         <v>287</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>1068</v>
+        <v>902</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>596</v>
@@ -7963,10 +7549,10 @@
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>1118</v>
+        <v>952</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>1095</v>
+        <v>929</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>288</v>
@@ -7975,7 +7561,7 @@
         <v>289</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>1069</v>
+        <v>903</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>597</v>
@@ -7998,10 +7584,10 @@
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>1119</v>
+        <v>953</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>1096</v>
+        <v>930</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>290</v>
@@ -8010,7 +7596,7 @@
         <v>291</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>1070</v>
+        <v>904</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>598</v>
@@ -8033,10 +7619,10 @@
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>1120</v>
+        <v>954</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>1097</v>
+        <v>931</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>292</v>
@@ -8045,7 +7631,7 @@
         <v>293</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>1071</v>
+        <v>905</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>599</v>
@@ -8068,10 +7654,10 @@
     </row>
     <row r="12" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>1121</v>
+        <v>955</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>1098</v>
+        <v>932</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>294</v>
@@ -8080,7 +7666,7 @@
         <v>295</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>1072</v>
+        <v>906</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>600</v>
@@ -8103,10 +7689,10 @@
     </row>
     <row r="13" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>1122</v>
+        <v>956</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>1099</v>
+        <v>933</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>296</v>
@@ -8115,7 +7701,7 @@
         <v>297</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>1073</v>
+        <v>907</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>601</v>
@@ -8138,10 +7724,10 @@
     </row>
     <row r="14" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>1123</v>
+        <v>957</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>1100</v>
+        <v>934</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>298</v>
@@ -8150,7 +7736,7 @@
         <v>299</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>1074</v>
+        <v>908</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>602</v>
@@ -8173,10 +7759,10 @@
     </row>
     <row r="15" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>1124</v>
+        <v>958</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>1101</v>
+        <v>935</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>300</v>
@@ -8185,7 +7771,7 @@
         <v>301</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>1075</v>
+        <v>909</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>603</v>
@@ -8208,10 +7794,10 @@
     </row>
     <row r="16" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>1125</v>
+        <v>959</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>1102</v>
+        <v>936</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>302</v>
@@ -8220,7 +7806,7 @@
         <v>303</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>1076</v>
+        <v>910</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>604</v>
@@ -8243,10 +7829,10 @@
     </row>
     <row r="17" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>1126</v>
+        <v>960</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>1103</v>
+        <v>937</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>304</v>
@@ -8255,7 +7841,7 @@
         <v>305</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>1077</v>
+        <v>911</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>605</v>
@@ -8278,10 +7864,10 @@
     </row>
     <row r="18" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>1127</v>
+        <v>961</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>1104</v>
+        <v>938</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>306</v>
@@ -8290,7 +7876,7 @@
         <v>307</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>1078</v>
+        <v>912</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>606</v>
@@ -8313,10 +7899,10 @@
     </row>
     <row r="19" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>1128</v>
+        <v>962</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>1105</v>
+        <v>939</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>308</v>
@@ -8325,7 +7911,7 @@
         <v>309</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>1079</v>
+        <v>913</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>607</v>
@@ -8348,10 +7934,10 @@
     </row>
     <row r="20" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>1129</v>
+        <v>963</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>1106</v>
+        <v>940</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>310</v>
@@ -8360,7 +7946,7 @@
         <v>311</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>1080</v>
+        <v>914</v>
       </c>
       <c r="F20" s="18" t="s">
         <v>608</v>
@@ -8383,10 +7969,10 @@
     </row>
     <row r="21" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>1130</v>
+        <v>964</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>1107</v>
+        <v>941</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>313</v>
@@ -8395,7 +7981,7 @@
         <v>314</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>1081</v>
+        <v>915</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>609</v>
@@ -8418,10 +8004,10 @@
     </row>
     <row r="22" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>1131</v>
+        <v>965</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>1108</v>
+        <v>942</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>315</v>
@@ -8430,7 +8016,7 @@
         <v>316</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>1082</v>
+        <v>916</v>
       </c>
       <c r="F22" s="18" t="s">
         <v>610</v>
@@ -8456,7 +8042,7 @@
         <v>317</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>1109</v>
+        <v>943</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>318</v>
@@ -8465,7 +8051,7 @@
         <v>319</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>1083</v>
+        <v>917</v>
       </c>
       <c r="F23" s="18" t="s">
         <v>611</v>
@@ -8488,10 +8074,10 @@
     </row>
     <row r="24" spans="1:11" s="5" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>1008</v>
+        <v>842</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>1110</v>
+        <v>944</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>318</v>
@@ -8500,7 +8086,7 @@
         <v>319</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>1132</v>
+        <v>966</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>611</v>
@@ -11804,7 +11390,7 @@
         <v>322</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>1192</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -12025,10 +11611,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337AF865-08E8-4C8C-A074-848D6C202917}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12038,7 +11624,10 @@
     <col min="3" max="3" width="76.140625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12050,2402 +11639,1024 @@
         <v>755</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>831</v>
+        <v>756</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>1193</v>
+        <v>1027</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>752</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>841</v>
+        <v>766</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>1195</v>
+        <v>1062</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>1194</v>
+        <v>1028</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>1199</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1201</v>
+      <c r="A2" s="2" t="s">
+        <v>1031</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>842</v>
+        <v>767</v>
       </c>
       <c r="C2" t="s">
-        <v>848</v>
+        <v>773</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>832</v>
+        <v>757</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F2" s="8">
-        <v>14.25</v>
+        <v>100</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>849</v>
-      </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="2">
-        <v>6</v>
+        <v>774</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>772</v>
       </c>
       <c r="J2" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1202</v>
+      <c r="A3" s="2" t="s">
+        <v>1032</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>843</v>
+        <v>768</v>
       </c>
       <c r="C3" t="s">
-        <v>928</v>
+        <v>807</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>833</v>
+        <v>758</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F3" s="2">
-        <v>10.25</v>
+        <v>805</v>
+      </c>
+      <c r="F3" s="8">
+        <v>150.5</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>850</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>1196</v>
-      </c>
-      <c r="I3" s="2">
-        <v>6</v>
+        <v>775</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>772</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>742</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>756</v>
+      <c r="A4" s="2" t="s">
+        <v>1033</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>844</v>
+        <v>769</v>
       </c>
       <c r="C4" t="s">
-        <v>929</v>
+        <v>808</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>834</v>
+        <v>759</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F4" s="8">
-        <v>14</v>
+        <v>2000</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>851</v>
-      </c>
-      <c r="H4" s="8"/>
+        <v>776</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1064</v>
+      </c>
       <c r="I4" s="2" t="s">
-        <v>847</v>
+        <v>772</v>
       </c>
       <c r="J4" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>757</v>
+      <c r="A5" s="2" t="s">
+        <v>1034</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>845</v>
+        <v>770</v>
       </c>
       <c r="C5" t="s">
-        <v>930</v>
+        <v>809</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>835</v>
+        <v>760</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F5" s="8">
-        <v>17</v>
+        <v>2100.5</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>852</v>
-      </c>
-      <c r="H5" s="8"/>
+        <v>777</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>1064</v>
+      </c>
       <c r="I5" s="2" t="s">
-        <v>847</v>
+        <v>772</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>742</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>758</v>
+      <c r="A6" s="2" t="s">
+        <v>1035</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>846</v>
+        <v>771</v>
       </c>
       <c r="C6" t="s">
-        <v>931</v>
+        <v>810</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>836</v>
+        <v>761</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F6" s="8">
-        <v>14.25</v>
+        <v>30000</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>853</v>
-      </c>
-      <c r="H6" s="8"/>
+        <v>778</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>1064</v>
+      </c>
       <c r="I6" s="2" t="s">
-        <v>847</v>
+        <v>772</v>
       </c>
       <c r="J6" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>759</v>
+      <c r="A7" s="2" t="s">
+        <v>1036</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>842</v>
+        <v>767</v>
       </c>
       <c r="C7" t="s">
-        <v>932</v>
+        <v>811</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>837</v>
+        <v>762</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F7" s="8">
-        <v>14.25</v>
+        <v>31000.134999999998</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>854</v>
-      </c>
-      <c r="H7" s="8"/>
+        <v>779</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>1064</v>
+      </c>
       <c r="I7" s="2" t="s">
-        <v>847</v>
+        <v>772</v>
       </c>
       <c r="J7" s="37" t="s">
-        <v>742</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>760</v>
+      <c r="A8" s="2" t="s">
+        <v>1037</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>843</v>
+        <v>768</v>
       </c>
       <c r="C8" t="s">
-        <v>933</v>
+        <v>812</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>838</v>
+        <v>763</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F8" s="2">
-        <v>10.25</v>
+        <v>805</v>
+      </c>
+      <c r="F8" s="8">
+        <v>350000.054</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>855</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>1197</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>847</v>
+        <v>780</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I8" s="8">
+        <v>10</v>
       </c>
       <c r="J8" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>761</v>
+      <c r="A9" s="2" t="s">
+        <v>1038</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>844</v>
+        <v>769</v>
       </c>
       <c r="C9" t="s">
-        <v>934</v>
+        <v>813</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>839</v>
+        <v>764</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F9" s="8">
-        <v>14</v>
+        <v>5510.5</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>856</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="2" t="s">
-        <v>847</v>
+        <v>781</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I9" s="8">
+        <v>10</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>742</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>762</v>
+      <c r="A10" s="2" t="s">
+        <v>1039</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>845</v>
+        <v>770</v>
       </c>
       <c r="C10" t="s">
-        <v>935</v>
+        <v>814</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>840</v>
+        <v>765</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F10" s="8">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>857</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="2" t="s">
-        <v>847</v>
+        <v>782</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I10" s="8">
+        <v>10</v>
       </c>
       <c r="J10" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>763</v>
+      <c r="A11" s="2" t="s">
+        <v>1040</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>846</v>
+        <v>771</v>
       </c>
       <c r="C11" t="s">
-        <v>936</v>
+        <v>815</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>631</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F11" s="8">
-        <v>14.25</v>
+        <v>1</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>858</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="2" t="s">
-        <v>847</v>
+        <v>783</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I11" s="8">
+        <v>10</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>742</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>764</v>
+      <c r="A12" s="2" t="s">
+        <v>1041</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>842</v>
+        <v>767</v>
       </c>
       <c r="C12" t="s">
-        <v>937</v>
+        <v>816</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>632</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F12" s="8">
-        <v>14.25</v>
+        <v>2000</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>859</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="2" t="s">
-        <v>847</v>
+        <v>784</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I12" s="8">
+        <v>10</v>
       </c>
       <c r="J12" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>765</v>
+      <c r="A13" s="2" t="s">
+        <v>1042</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>843</v>
+        <v>768</v>
       </c>
       <c r="C13" t="s">
-        <v>938</v>
+        <v>817</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>633</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F13" s="2">
-        <v>10.25</v>
+        <v>805</v>
+      </c>
+      <c r="F13" s="8">
+        <v>640.5</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>860</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>1198</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>847</v>
+        <v>785</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I13" s="8">
+        <v>10</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>742</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>766</v>
+      <c r="A14" s="2" t="s">
+        <v>1043</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>844</v>
+        <v>769</v>
       </c>
       <c r="C14" t="s">
-        <v>939</v>
+        <v>818</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>634</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F14" s="8">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>861</v>
-      </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="2" t="s">
-        <v>847</v>
+        <v>786</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>767</v>
+      <c r="A15" s="2" t="s">
+        <v>1044</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>845</v>
+        <v>770</v>
       </c>
       <c r="C15" t="s">
-        <v>940</v>
+        <v>819</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>635</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F15" s="8">
-        <v>17</v>
+        <v>150.5</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>862</v>
-      </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="2" t="s">
-        <v>847</v>
+        <v>787</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
       </c>
       <c r="J15" s="37" t="s">
-        <v>742</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>768</v>
+      <c r="A16" s="2" t="s">
+        <v>1045</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>846</v>
+        <v>771</v>
       </c>
       <c r="C16" t="s">
-        <v>941</v>
+        <v>820</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>636</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F16" s="8">
-        <v>14.25</v>
+        <v>2000</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>863</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="2" t="s">
-        <v>847</v>
+        <v>788</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
       </c>
       <c r="J16" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>769</v>
+      <c r="A17" s="2" t="s">
+        <v>1046</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>842</v>
+        <v>767</v>
       </c>
       <c r="C17" t="s">
-        <v>942</v>
+        <v>821</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>637</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>926</v>
+        <v>805</v>
       </c>
       <c r="F17" s="8">
-        <v>14.25</v>
+        <v>2100.5</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>864</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="2" t="s">
-        <v>847</v>
+        <v>789</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
       </c>
       <c r="J17" s="37" t="s">
-        <v>742</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>770</v>
+      <c r="A18" s="2" t="s">
+        <v>1047</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>843</v>
+        <v>768</v>
       </c>
       <c r="C18" t="s">
-        <v>943</v>
+        <v>822</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>638</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F18" s="2">
-        <v>10.25</v>
+        <v>805</v>
+      </c>
+      <c r="F18" s="8">
+        <v>30000</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>865</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>1196</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>847</v>
+        <v>790</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
       </c>
       <c r="J18" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>771</v>
+      <c r="A19" s="2" t="s">
+        <v>1048</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>844</v>
+        <v>769</v>
       </c>
       <c r="C19" t="s">
-        <v>944</v>
+        <v>823</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>639</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F19" s="8">
-        <v>14</v>
+        <v>31000.134999999998</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>866</v>
-      </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="2" t="s">
-        <v>847</v>
+        <v>791</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0</v>
       </c>
       <c r="J19" s="37" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>772</v>
+      <c r="A20" s="2" t="s">
+        <v>1049</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>845</v>
+        <v>770</v>
       </c>
       <c r="C20" t="s">
-        <v>945</v>
+        <v>824</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>640</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F20" s="8">
-        <v>17</v>
+        <v>350000.054</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>867</v>
-      </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8">
-        <v>1000</v>
-      </c>
+        <v>792</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I20" s="8"/>
       <c r="J20" s="37" t="s">
-        <v>743</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>773</v>
+      <c r="A21" s="2" t="s">
+        <v>1050</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>846</v>
+        <v>771</v>
       </c>
       <c r="C21" t="s">
-        <v>946</v>
+        <v>825</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>641</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F21" s="8">
-        <v>14.25</v>
+        <v>5510.5</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>868</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8">
-        <v>1000</v>
-      </c>
+        <v>793</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I21" s="8"/>
       <c r="J21" s="37" t="s">
-        <v>1200</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>774</v>
+      <c r="A22" s="2" t="s">
+        <v>1051</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>842</v>
+        <v>767</v>
       </c>
       <c r="C22" t="s">
-        <v>947</v>
+        <v>826</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>642</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F22" s="8">
-        <v>14.25</v>
+        <v>10</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>869</v>
-      </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="2" t="s">
-        <v>847</v>
-      </c>
+        <v>794</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I22" s="2"/>
       <c r="J22" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>775</v>
+      <c r="A23" s="2" t="s">
+        <v>1052</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>843</v>
+        <v>768</v>
       </c>
       <c r="C23" t="s">
-        <v>948</v>
+        <v>827</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>643</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F23" s="2">
-        <v>10.25</v>
+        <v>806</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>870</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>1197</v>
-      </c>
-      <c r="I23" s="8">
-        <v>1000</v>
-      </c>
+        <v>795</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I23" s="8"/>
       <c r="J23" s="37" t="s">
-        <v>1200</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>776</v>
+      <c r="A24" s="2" t="s">
+        <v>1053</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>844</v>
+        <v>769</v>
       </c>
       <c r="C24" t="s">
-        <v>949</v>
+        <v>828</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>644</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F24" s="8">
-        <v>14</v>
+        <v>2000</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>871</v>
-      </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="2" t="s">
-        <v>847</v>
-      </c>
+        <v>796</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I24" s="2"/>
       <c r="J24" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>777</v>
+      <c r="A25" s="2" t="s">
+        <v>1054</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>845</v>
+        <v>770</v>
       </c>
       <c r="C25" t="s">
-        <v>950</v>
+        <v>829</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>645</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F25" s="8">
-        <v>17</v>
+        <v>640.5</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>872</v>
-      </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8">
-        <v>1000</v>
-      </c>
+        <v>797</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I25" s="8"/>
       <c r="J25" s="37" t="s">
         <v>743</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>778</v>
+      <c r="A26" s="2" t="s">
+        <v>1055</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>846</v>
+        <v>771</v>
       </c>
       <c r="C26" t="s">
-        <v>951</v>
+        <v>830</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>646</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F26" s="8">
-        <v>14.25</v>
+        <v>100</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>873</v>
-      </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8">
-        <v>1000</v>
-      </c>
+        <v>798</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I26" s="8"/>
       <c r="J26" s="37" t="s">
-        <v>1200</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>779</v>
+      <c r="A27" s="2" t="s">
+        <v>1056</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>842</v>
+        <v>767</v>
       </c>
       <c r="C27" t="s">
-        <v>952</v>
+        <v>831</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>647</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F27" s="8">
-        <v>14.25</v>
+        <v>150.5</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>874</v>
-      </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="2" t="s">
-        <v>847</v>
-      </c>
+        <v>799</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I27" s="2"/>
       <c r="J27" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>780</v>
+      <c r="A28" s="2" t="s">
+        <v>1057</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>843</v>
+        <v>768</v>
       </c>
       <c r="C28" t="s">
-        <v>953</v>
+        <v>832</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>648</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F28" s="2">
-        <v>10.25</v>
+        <v>806</v>
+      </c>
+      <c r="F28" s="8">
+        <v>2000</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>875</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>1198</v>
-      </c>
-      <c r="I28" s="8">
-        <v>1000</v>
-      </c>
+        <v>800</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I28" s="8"/>
       <c r="J28" s="37" t="s">
-        <v>1200</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>781</v>
+      <c r="A29" s="2" t="s">
+        <v>1058</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>844</v>
+        <v>769</v>
       </c>
       <c r="C29" t="s">
-        <v>954</v>
+        <v>833</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>649</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F29" s="8">
-        <v>14</v>
+        <v>2100.5</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>876</v>
-      </c>
-      <c r="H29" s="8"/>
-      <c r="I29" s="2" t="s">
-        <v>847</v>
-      </c>
+        <v>801</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I29" s="2"/>
       <c r="J29" s="37" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>782</v>
+      <c r="A30" s="2" t="s">
+        <v>1059</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>845</v>
+        <v>770</v>
       </c>
       <c r="C30" t="s">
-        <v>955</v>
+        <v>834</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>650</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F30" s="8">
-        <v>17</v>
+        <v>30000</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>877</v>
-      </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8">
-        <v>1000</v>
-      </c>
+        <v>802</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I30" s="8"/>
       <c r="J30" s="37" t="s">
         <v>743</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>783</v>
+      <c r="A31" s="2" t="s">
+        <v>1060</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>846</v>
+        <v>771</v>
       </c>
       <c r="C31" t="s">
-        <v>956</v>
+        <v>835</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>651</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F31" s="8">
-        <v>14.25</v>
+        <v>31000.134999999998</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>878</v>
-      </c>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8">
-        <v>1000</v>
-      </c>
+        <v>803</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I31" s="8"/>
       <c r="J31" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>784</v>
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>1061</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>842</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>957</v>
+        <v>836</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>652</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>926</v>
+        <v>806</v>
       </c>
       <c r="F32" s="8">
-        <v>14.25</v>
+        <v>100</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>879</v>
-      </c>
-      <c r="H32" s="8"/>
-      <c r="I32" s="2" t="s">
-        <v>847</v>
-      </c>
+        <v>804</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I32" s="2"/>
       <c r="J32" s="37" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>785</v>
+        <v>838</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>843</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>958</v>
+        <v>837</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>653</v>
+        <v>838</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F33" s="2">
-        <v>10.25</v>
+        <v>806</v>
+      </c>
+      <c r="F33" s="8">
+        <v>150.5</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>880</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>1196</v>
-      </c>
-      <c r="I33" s="8">
-        <v>1000</v>
-      </c>
+        <v>839</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I33" s="2"/>
       <c r="J33" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>786</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C34" t="s">
-        <v>959</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F34" s="8">
-        <v>14</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>881</v>
-      </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J34" s="37" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="C35" t="s">
-        <v>960</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F35" s="8">
-        <v>17</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>882</v>
-      </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8">
-        <v>1000</v>
-      </c>
-      <c r="J35" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>788</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="C36" t="s">
-        <v>961</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F36" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>883</v>
-      </c>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8">
-        <v>1000</v>
-      </c>
-      <c r="J36" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>789</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C37" t="s">
-        <v>962</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F37" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>884</v>
-      </c>
-      <c r="H37" s="8"/>
-      <c r="I37" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J37" s="37" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>790</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>843</v>
-      </c>
-      <c r="C38" t="s">
-        <v>963</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F38" s="2">
-        <v>10.25</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>885</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>1197</v>
-      </c>
-      <c r="I38" s="2">
-        <v>0</v>
-      </c>
-      <c r="J38" s="37" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>791</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C39" t="s">
-        <v>964</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F39" s="8">
-        <v>14</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>886</v>
-      </c>
-      <c r="H39" s="8"/>
-      <c r="I39" s="2">
-        <v>0</v>
-      </c>
-      <c r="J39" s="37" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>792</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="C40" t="s">
-        <v>965</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F40" s="8">
-        <v>17</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>887</v>
-      </c>
-      <c r="H40" s="8"/>
-      <c r="I40" s="2">
-        <v>0</v>
-      </c>
-      <c r="J40" s="37" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>793</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="C41" t="s">
-        <v>966</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F41" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>888</v>
-      </c>
-      <c r="H41" s="8"/>
-      <c r="I41" s="2">
-        <v>0</v>
-      </c>
-      <c r="J41" s="37" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>794</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C42" t="s">
-        <v>967</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F42" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>889</v>
-      </c>
-      <c r="H42" s="8"/>
-      <c r="I42" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J42" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>795</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>843</v>
-      </c>
-      <c r="C43" t="s">
-        <v>968</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F43" s="2">
-        <v>10.25</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>890</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>1198</v>
-      </c>
-      <c r="I43" s="2">
-        <v>0</v>
-      </c>
-      <c r="J43" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C44" t="s">
-        <v>969</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F44" s="8">
-        <v>14</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>891</v>
-      </c>
-      <c r="H44" s="8"/>
-      <c r="I44" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J44" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>797</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="C45" t="s">
-        <v>930</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F45" s="8">
-        <v>17</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>892</v>
-      </c>
-      <c r="H45" s="8"/>
-      <c r="I45" s="2">
-        <v>0</v>
-      </c>
-      <c r="J45" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>798</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="C46" t="s">
-        <v>970</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F46" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>893</v>
-      </c>
-      <c r="H46" s="8"/>
-      <c r="I46" s="2">
-        <v>0</v>
-      </c>
-      <c r="J46" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>799</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C47" t="s">
-        <v>971</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F47" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>894</v>
-      </c>
-      <c r="H47" s="8"/>
-      <c r="I47" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J47" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>800</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>843</v>
-      </c>
-      <c r="C48" t="s">
-        <v>972</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>668</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F48" s="2">
-        <v>10.25</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>895</v>
-      </c>
-      <c r="H48" s="8" t="s">
-        <v>1196</v>
-      </c>
-      <c r="I48" s="2">
-        <v>0</v>
-      </c>
-      <c r="J48" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>801</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C49" t="s">
-        <v>973</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F49" s="8">
-        <v>14</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>896</v>
-      </c>
-      <c r="H49" s="8"/>
-      <c r="I49" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J49" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>802</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="C50" t="s">
-        <v>974</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>670</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F50" s="8">
-        <v>17</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>897</v>
-      </c>
-      <c r="H50" s="8"/>
-      <c r="I50" s="2">
-        <v>0</v>
-      </c>
-      <c r="J50" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="C51" t="s">
-        <v>975</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F51" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>898</v>
-      </c>
-      <c r="H51" s="8"/>
-      <c r="I51" s="2">
-        <v>0</v>
-      </c>
-      <c r="J51" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>804</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C52" t="s">
-        <v>976</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F52" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>899</v>
-      </c>
-      <c r="H52" s="8"/>
-      <c r="I52" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J52" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>843</v>
-      </c>
-      <c r="C53" t="s">
-        <v>977</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F53" s="2">
-        <v>10.25</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>900</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>1197</v>
-      </c>
-      <c r="I53" s="2">
-        <v>0</v>
-      </c>
-      <c r="J53" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>806</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C54" t="s">
-        <v>978</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F54" s="8">
-        <v>14</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>901</v>
-      </c>
-      <c r="H54" s="8"/>
-      <c r="I54" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J54" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>807</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="C55" t="s">
-        <v>979</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F55" s="8">
-        <v>17</v>
-      </c>
-      <c r="G55" s="8" t="s">
-        <v>902</v>
-      </c>
-      <c r="H55" s="8"/>
-      <c r="I55" s="2">
-        <v>0</v>
-      </c>
-      <c r="J55" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="C56" t="s">
-        <v>980</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>676</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F56" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>903</v>
-      </c>
-      <c r="H56" s="8"/>
-      <c r="I56" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J56" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>809</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C57" t="s">
-        <v>981</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F57" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G57" s="8" t="s">
-        <v>904</v>
-      </c>
-      <c r="H57" s="8"/>
-      <c r="I57" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J57" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>810</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>843</v>
-      </c>
-      <c r="C58" t="s">
-        <v>982</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F58" s="2">
-        <v>10.25</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>905</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>1198</v>
-      </c>
-      <c r="I58" s="2">
-        <v>0</v>
-      </c>
-      <c r="J58" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>811</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C59" t="s">
-        <v>983</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F59" s="8">
-        <v>14</v>
-      </c>
-      <c r="G59" s="8" t="s">
-        <v>906</v>
-      </c>
-      <c r="H59" s="8"/>
-      <c r="I59" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J59" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>812</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="C60" t="s">
-        <v>984</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F60" s="8">
-        <v>17</v>
-      </c>
-      <c r="G60" s="8" t="s">
-        <v>907</v>
-      </c>
-      <c r="H60" s="8"/>
-      <c r="I60" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J60" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>813</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="C61" t="s">
-        <v>985</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F61" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G61" s="8" t="s">
-        <v>908</v>
-      </c>
-      <c r="H61" s="8"/>
-      <c r="I61" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J61" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C62" t="s">
-        <v>986</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F62" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G62" s="8" t="s">
-        <v>909</v>
-      </c>
-      <c r="H62" s="8"/>
-      <c r="I62" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J62" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>843</v>
-      </c>
-      <c r="C63" t="s">
-        <v>987</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F63" s="2">
-        <v>10.25</v>
-      </c>
-      <c r="G63" s="8" t="s">
-        <v>910</v>
-      </c>
-      <c r="H63" s="8" t="s">
-        <v>1196</v>
-      </c>
-      <c r="I63" s="2">
-        <v>0</v>
-      </c>
-      <c r="J63" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C64" t="s">
-        <v>988</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F64" s="8">
-        <v>14</v>
-      </c>
-      <c r="G64" s="8" t="s">
-        <v>911</v>
-      </c>
-      <c r="H64" s="8"/>
-      <c r="I64" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J64" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="C65" t="s">
-        <v>989</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F65" s="8">
-        <v>17</v>
-      </c>
-      <c r="G65" s="8" t="s">
-        <v>912</v>
-      </c>
-      <c r="H65" s="8"/>
-      <c r="I65" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J65" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="C66" t="s">
-        <v>990</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F66" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G66" s="8" t="s">
-        <v>913</v>
-      </c>
-      <c r="H66" s="8"/>
-      <c r="I66" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J66" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C67" t="s">
-        <v>991</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F67" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>914</v>
-      </c>
-      <c r="H67" s="8"/>
-      <c r="I67" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J67" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>820</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>843</v>
-      </c>
-      <c r="C68" t="s">
-        <v>992</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F68" s="2">
-        <v>10.25</v>
-      </c>
-      <c r="G68" s="8" t="s">
-        <v>915</v>
-      </c>
-      <c r="H68" s="8" t="s">
-        <v>1197</v>
-      </c>
-      <c r="I68" s="2">
-        <v>0</v>
-      </c>
-      <c r="J68" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C69" t="s">
-        <v>993</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F69" s="8">
-        <v>14</v>
-      </c>
-      <c r="G69" s="8" t="s">
-        <v>916</v>
-      </c>
-      <c r="H69" s="8"/>
-      <c r="I69" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J69" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="C70" t="s">
-        <v>994</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F70" s="8">
-        <v>17</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>917</v>
-      </c>
-      <c r="H70" s="8"/>
-      <c r="I70" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J70" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="C71" t="s">
-        <v>995</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F71" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>918</v>
-      </c>
-      <c r="H71" s="8"/>
-      <c r="I71" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J71" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>824</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C72" t="s">
-        <v>996</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F72" s="8">
-        <v>14.25</v>
-      </c>
-      <c r="G72" s="8" t="s">
-        <v>919</v>
-      </c>
-      <c r="H72" s="8"/>
-      <c r="I72" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J72" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>843</v>
-      </c>
-      <c r="C73" t="s">
-        <v>997</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F73" s="2">
-        <v>10.25</v>
-      </c>
-      <c r="G73" s="8" t="s">
-        <v>920</v>
-      </c>
-      <c r="H73" s="8" t="s">
-        <v>1198</v>
-      </c>
-      <c r="I73" s="2">
-        <v>0</v>
-      </c>
-      <c r="J73" s="37" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>826</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="C74" t="s">
-        <v>998</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>694</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F74" s="8">
-        <v>15</v>
-      </c>
-      <c r="G74" s="8" t="s">
-        <v>921</v>
-      </c>
-      <c r="H74" s="8"/>
-      <c r="I74" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J74" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>827</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C75" t="s">
-        <v>999</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F75" s="8">
-        <v>15</v>
-      </c>
-      <c r="G75" s="8" t="s">
-        <v>922</v>
-      </c>
-      <c r="H75" s="8"/>
-      <c r="I75" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J75" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
-        <v>828</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C76" t="s">
-        <v>1000</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F76" s="8">
-        <v>15</v>
-      </c>
-      <c r="G76" s="8" t="s">
-        <v>923</v>
-      </c>
-      <c r="H76" s="8"/>
-      <c r="I76" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J76" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>829</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="C77" t="s">
-        <v>1001</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F77" s="8">
-        <v>15</v>
-      </c>
-      <c r="G77" s="8" t="s">
-        <v>924</v>
-      </c>
-      <c r="H77" s="8"/>
-      <c r="I77" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J77" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>830</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C78" t="s">
-        <v>1002</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F78" s="8">
-        <v>15</v>
-      </c>
-      <c r="G78" s="8" t="s">
-        <v>925</v>
-      </c>
-      <c r="H78" s="8" t="s">
-        <v>1198</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J78" s="37" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
-        <v>1003</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C79" t="s">
-        <v>1004</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>927</v>
-      </c>
-      <c r="F79" s="8">
-        <v>15</v>
-      </c>
-      <c r="G79" s="8" t="s">
-        <v>1005</v>
-      </c>
-      <c r="H79" s="8" t="s">
-        <v>1198</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="J79" s="37" t="s">
-        <v>1200</v>
+        <v>1030</v>
       </c>
     </row>
   </sheetData>
@@ -14488,111 +12699,111 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1009</v>
+        <v>843</v>
       </c>
       <c r="B1" t="s">
-        <v>1010</v>
+        <v>844</v>
       </c>
       <c r="C1" t="s">
-        <v>1011</v>
+        <v>845</v>
       </c>
       <c r="D1" t="s">
-        <v>1012</v>
+        <v>846</v>
       </c>
       <c r="E1" t="s">
-        <v>1013</v>
+        <v>847</v>
       </c>
       <c r="F1" t="s">
-        <v>1014</v>
+        <v>848</v>
       </c>
       <c r="G1" t="s">
-        <v>1015</v>
+        <v>849</v>
       </c>
       <c r="H1" t="s">
         <v>123</v>
       </c>
       <c r="I1" t="s">
-        <v>1016</v>
+        <v>850</v>
       </c>
       <c r="J1" t="s">
-        <v>1017</v>
+        <v>851</v>
       </c>
       <c r="K1" t="s">
-        <v>1018</v>
+        <v>852</v>
       </c>
       <c r="L1" t="s">
-        <v>1019</v>
+        <v>853</v>
       </c>
       <c r="M1" t="s">
-        <v>1020</v>
+        <v>854</v>
       </c>
       <c r="N1" t="s">
         <v>731</v>
       </c>
       <c r="O1" t="s">
-        <v>1021</v>
+        <v>855</v>
       </c>
       <c r="P1" t="s">
-        <v>1022</v>
+        <v>856</v>
       </c>
       <c r="Q1" t="s">
-        <v>1023</v>
+        <v>857</v>
       </c>
       <c r="R1" t="s">
-        <v>1024</v>
+        <v>858</v>
       </c>
       <c r="S1" t="s">
-        <v>1025</v>
+        <v>859</v>
       </c>
       <c r="T1" t="s">
-        <v>1026</v>
+        <v>860</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1027</v>
+        <v>861</v>
       </c>
       <c r="B2" t="s">
-        <v>1028</v>
+        <v>862</v>
       </c>
       <c r="C2" t="s">
-        <v>1029</v>
+        <v>863</v>
       </c>
       <c r="H2" t="s">
-        <v>1030</v>
+        <v>864</v>
       </c>
       <c r="I2" t="s">
-        <v>1031</v>
+        <v>865</v>
       </c>
       <c r="J2" t="s">
-        <v>1032</v>
+        <v>866</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>1038</v>
+        <v>872</v>
       </c>
       <c r="L2" t="s">
-        <v>1029</v>
+        <v>863</v>
       </c>
       <c r="M2" t="s">
-        <v>1033</v>
+        <v>867</v>
       </c>
       <c r="N2" t="s">
-        <v>1034</v>
+        <v>868</v>
       </c>
       <c r="O2" t="s">
-        <v>1039</v>
+        <v>873</v>
       </c>
       <c r="P2" t="s">
-        <v>1040</v>
+        <v>874</v>
       </c>
       <c r="Q2" t="s">
-        <v>1035</v>
+        <v>869</v>
       </c>
       <c r="R2" t="s">
-        <v>1036</v>
+        <v>870</v>
       </c>
       <c r="S2" t="s">
-        <v>1037</v>
+        <v>871</v>
       </c>
       <c r="T2">
         <v>20</v>

</xml_diff>

<commit_message>
Commit for Checkout SUPEBABY
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Admin Category" sheetId="1" state="visible" r:id="rId2"/>
@@ -2819,25 +2819,7 @@
     <t xml:space="preserve">multiplecategory</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item2.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item2.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Description02</t>
@@ -2855,25 +2837,7 @@
     <t xml:space="preserve">category1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item3.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item3.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Description03</t>
@@ -2888,25 +2852,7 @@
     <t xml:space="preserve">category2.1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item4.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item4.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Description04</t>
@@ -2921,25 +2867,7 @@
     <t xml:space="preserve">category3.1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item5.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item5.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Description05</t>
@@ -2951,25 +2879,7 @@
     <t xml:space="preserve">Item_06</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item6.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item6.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Description06</t>
@@ -2981,25 +2891,7 @@
     <t xml:space="preserve">Item_07</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item7.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item7.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Description07</t>
@@ -3011,25 +2903,7 @@
     <t xml:space="preserve">Item_08</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item8.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item8.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Description08</t>
@@ -3041,25 +2915,7 @@
     <t xml:space="preserve">Item_09</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item9.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item9.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Description09</t>
@@ -3071,25 +2927,7 @@
     <t xml:space="preserve">Item_10</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item10.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item10.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU010</t>
@@ -3098,25 +2936,7 @@
     <t xml:space="preserve">Item_11</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item11.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item11.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU011</t>
@@ -3125,25 +2945,7 @@
     <t xml:space="preserve">Item_12</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item12.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item12.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU012</t>
@@ -3152,25 +2954,7 @@
     <t xml:space="preserve">Item_13</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item13.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item13.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU013</t>
@@ -3179,25 +2963,7 @@
     <t xml:space="preserve">Item_14</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item14.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item14.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU014</t>
@@ -3206,25 +2972,7 @@
     <t xml:space="preserve">Item_15</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item15.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item15.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU015</t>
@@ -3233,25 +2981,7 @@
     <t xml:space="preserve">Item_16</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item16.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item16.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU016</t>
@@ -3260,25 +2990,7 @@
     <t xml:space="preserve">Item_17</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item17.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item17.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU017</t>
@@ -3287,25 +2999,7 @@
     <t xml:space="preserve">Item_18</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item18.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item18.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -3317,25 +3011,7 @@
     <t xml:space="preserve">Item_19</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item19.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item19.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU019</t>
@@ -3347,25 +3023,7 @@
     <t xml:space="preserve">Item_20</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item20.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item20.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU020</t>
@@ -3374,25 +3032,7 @@
     <t xml:space="preserve">Item_21</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item21.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item21.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU021</t>
@@ -3401,25 +3041,7 @@
     <t xml:space="preserve">Item_22</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item22.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item22.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU022</t>
@@ -3428,25 +3050,7 @@
     <t xml:space="preserve">Item_23</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item23.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item23.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU023</t>
@@ -3455,25 +3059,7 @@
     <t xml:space="preserve">Item_24</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item24.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item24.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU024</t>
@@ -3482,25 +3068,7 @@
     <t xml:space="preserve">Item_25</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item25.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item25.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU025</t>
@@ -3509,25 +3077,7 @@
     <t xml:space="preserve">Item_26</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item26.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item26.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU026</t>
@@ -3536,25 +3086,7 @@
     <t xml:space="preserve">Item_27</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item27.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item27.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU027</t>
@@ -3563,25 +3095,7 @@
     <t xml:space="preserve">Item_28</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item28.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item28.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU028</t>
@@ -3590,25 +3104,7 @@
     <t xml:space="preserve">Item_29</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item29.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item29.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU029</t>
@@ -3617,25 +3113,7 @@
     <t xml:space="preserve">Item_30</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item30.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item30.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU030</t>
@@ -3644,25 +3122,7 @@
     <t xml:space="preserve">Item_31</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item31.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item31.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU077</t>
@@ -3671,25 +3131,7 @@
     <t xml:space="preserve">ITEM FOR EDIT</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">item32.jpg</t>
-    </r>
+    <t xml:space="preserve">C:\\Katalon\\BespokeAPI\\Images\\UN Items\\item32.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SKU078</t>
@@ -4249,7 +3691,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4271,12 +3713,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4435,7 +3871,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -4444,19 +3880,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4472,15 +3908,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4488,39 +3924,39 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4528,55 +3964,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4584,11 +4020,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4676,7 +4112,7 @@
       <selection pane="topLeft" activeCell="G72" activeCellId="0" sqref="G72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.43"/>
@@ -5806,85 +5242,85 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="\\Katalon\\BespokeAPI\\Images\\Category\\1.png"/>
-    <hyperlink ref="C3" r:id="rId2" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C4" r:id="rId3" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C5" r:id="rId4" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C6" r:id="rId5" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C7" r:id="rId6" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C8" r:id="rId7" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C9" r:id="rId8" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C10" r:id="rId9" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C11" r:id="rId10" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C12" r:id="rId11" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C13" r:id="rId12" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C14" r:id="rId13" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C15" r:id="rId14" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C16" r:id="rId15" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C17" r:id="rId16" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C18" r:id="rId17" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C19" r:id="rId18" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C20" r:id="rId19" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C21" r:id="rId20" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C22" r:id="rId21" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C23" r:id="rId22" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C24" r:id="rId23" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C25" r:id="rId24" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C26" r:id="rId25" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C27" r:id="rId26" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C28" r:id="rId27" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C29" r:id="rId28" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C30" r:id="rId29" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C31" r:id="rId30" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C32" r:id="rId31" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C33" r:id="rId32" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C34" r:id="rId33" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C35" r:id="rId34" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C36" r:id="rId35" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C37" r:id="rId36" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C38" r:id="rId37" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C39" r:id="rId38" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C40" r:id="rId39" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C41" r:id="rId40" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C42" r:id="rId41" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C43" r:id="rId42" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C44" r:id="rId43" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C45" r:id="rId44" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C46" r:id="rId45" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C47" r:id="rId46" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C48" r:id="rId47" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C49" r:id="rId48" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C50" r:id="rId49" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C51" r:id="rId50" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C52" r:id="rId51" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C53" r:id="rId52" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C54" r:id="rId53" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C55" r:id="rId54" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C56" r:id="rId55" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C57" r:id="rId56" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C58" r:id="rId57" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C59" r:id="rId58" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C60" r:id="rId59" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C61" r:id="rId60" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C62" r:id="rId61" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C63" r:id="rId62" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C64" r:id="rId63" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C65" r:id="rId64" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C66" r:id="rId65" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C67" r:id="rId66" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C68" r:id="rId67" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C69" r:id="rId68" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C70" r:id="rId69" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C71" r:id="rId70" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C72" r:id="rId71" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C73" r:id="rId72" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C74" r:id="rId73" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C75" r:id="rId74" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C76" r:id="rId75" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C77" r:id="rId76" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C78" r:id="rId77" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C79" r:id="rId78" display="\\Katalon\\BespokeAPI\\Images\\"/>
-    <hyperlink ref="C80" r:id="rId79" display="\\Katalon\\BespokeAPI\\Images\\"/>
+    <hyperlink ref="C2" r:id="rId1" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\1.png"/>
+    <hyperlink ref="C3" r:id="rId2" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\2.png"/>
+    <hyperlink ref="C4" r:id="rId3" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\2.png"/>
+    <hyperlink ref="C5" r:id="rId4" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\2.png"/>
+    <hyperlink ref="C6" r:id="rId5" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\3.png"/>
+    <hyperlink ref="C7" r:id="rId6" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\3.png"/>
+    <hyperlink ref="C8" r:id="rId7" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\3.png"/>
+    <hyperlink ref="C9" r:id="rId8" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\3.png"/>
+    <hyperlink ref="C10" r:id="rId9" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\3.png"/>
+    <hyperlink ref="C11" r:id="rId10" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C12" r:id="rId11" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C13" r:id="rId12" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C14" r:id="rId13" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C15" r:id="rId14" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C16" r:id="rId15" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C17" r:id="rId16" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C18" r:id="rId17" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C19" r:id="rId18" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C20" r:id="rId19" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C21" r:id="rId20" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C22" r:id="rId21" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C23" r:id="rId22" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C24" r:id="rId23" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C25" r:id="rId24" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C26" r:id="rId25" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C27" r:id="rId26" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C28" r:id="rId27" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C29" r:id="rId28" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C30" r:id="rId29" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C31" r:id="rId30" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\4.png"/>
+    <hyperlink ref="C32" r:id="rId31" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C33" r:id="rId32" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C34" r:id="rId33" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C35" r:id="rId34" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C36" r:id="rId35" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C37" r:id="rId36" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C38" r:id="rId37" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C39" r:id="rId38" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C40" r:id="rId39" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C41" r:id="rId40" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C42" r:id="rId41" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C43" r:id="rId42" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C44" r:id="rId43" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C45" r:id="rId44" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C46" r:id="rId45" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C47" r:id="rId46" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C48" r:id="rId47" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C49" r:id="rId48" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C50" r:id="rId49" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C51" r:id="rId50" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C52" r:id="rId51" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C53" r:id="rId52" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C54" r:id="rId53" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\5.png"/>
+    <hyperlink ref="C55" r:id="rId54" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\6.png"/>
+    <hyperlink ref="C56" r:id="rId55" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\6.png"/>
+    <hyperlink ref="C57" r:id="rId56" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\6.png"/>
+    <hyperlink ref="C58" r:id="rId57" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\6.png"/>
+    <hyperlink ref="C59" r:id="rId58" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\6.png"/>
+    <hyperlink ref="C60" r:id="rId59" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\6.png"/>
+    <hyperlink ref="C61" r:id="rId60" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\6.png"/>
+    <hyperlink ref="C62" r:id="rId61" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\6.png"/>
+    <hyperlink ref="C63" r:id="rId62" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\6.png"/>
+    <hyperlink ref="C64" r:id="rId63" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\7.png"/>
+    <hyperlink ref="C65" r:id="rId64" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\8.png"/>
+    <hyperlink ref="C66" r:id="rId65" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\9.png"/>
+    <hyperlink ref="C67" r:id="rId66" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\10.png"/>
+    <hyperlink ref="C68" r:id="rId67" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\11.png"/>
+    <hyperlink ref="C69" r:id="rId68" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\12.png"/>
+    <hyperlink ref="C70" r:id="rId69" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\13.png"/>
+    <hyperlink ref="C71" r:id="rId70" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\14.png"/>
+    <hyperlink ref="C72" r:id="rId71" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\15.png"/>
+    <hyperlink ref="C73" r:id="rId72" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\16.png"/>
+    <hyperlink ref="C74" r:id="rId73" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\17.png"/>
+    <hyperlink ref="C75" r:id="rId74" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\18.png"/>
+    <hyperlink ref="C76" r:id="rId75" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\19.png"/>
+    <hyperlink ref="C77" r:id="rId76" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\20.png"/>
+    <hyperlink ref="C78" r:id="rId77" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\21.png"/>
+    <hyperlink ref="C79" r:id="rId78" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\22.png"/>
+    <hyperlink ref="C80" r:id="rId79" display="C:\\Katalon\\BespokeAPI\\Images\\Category\\23.png"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5907,14 +5343,14 @@
       <selection pane="topLeft" activeCell="N25" activeCellId="0" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.99"/>
@@ -6060,24 +5496,24 @@
   </sheetPr>
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C84" activeCellId="0" sqref="C84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="76.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9365,12 +8801,12 @@
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="20.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="5" width="9.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="5" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10240,14 +9676,14 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="46.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="29.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="38.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="46.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="14.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="7" width="9.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="7" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10550,7 +9986,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="62.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.42"/>
@@ -11704,14 +11140,14 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.57"/>
@@ -12582,10 +12018,10 @@
       <selection pane="topLeft" activeCell="J30" activeCellId="0" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12725,11 +12161,11 @@
       <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.87"/>
   </cols>
@@ -15190,11 +14626,11 @@
   </sheetPr>
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q64" activeCellId="0" sqref="Q64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
@@ -15202,7 +14638,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
         <v>892</v>
       </c>
@@ -16235,12 +15671,12 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="76.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.87"/>

</xml_diff>